<commit_message>
Add inter/extrapolation rules to constraints (mostly)
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_PWR_RNW_Potentials.xlsx
+++ b/SuppXLS/Scen_PWR_RNW_Potentials.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD1D0CEA-FE38-4818-9DD8-BD4FF76EA280}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B3AC272-34A3-4536-99FD-6EEB4D3FA7B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3233" yWindow="8002" windowWidth="20716" windowHeight="13276" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="6" r:id="rId1"/>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="156">
   <si>
     <t>UC_N</t>
   </si>
@@ -154,15 +154,6 @@
   </si>
   <si>
     <t>IE</t>
-  </si>
-  <si>
-    <t>Pset_PD</t>
-  </si>
-  <si>
-    <t>Cset_Set</t>
-  </si>
-  <si>
-    <t>Cset_CD</t>
   </si>
   <si>
     <t>CAP_BND</t>
@@ -1327,7 +1318,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1384,6 +1375,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="40">
     <cellStyle name="20% - Accent1" xfId="17" builtinId="30" customBuiltin="1"/>
@@ -1513,13 +1508,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>501276</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>72167</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2037,13 +2032,13 @@
     </row>
     <row r="5" spans="1:30">
       <c r="A5" s="28" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C5" s="30" t="s">
         <v>25</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E5" s="29" t="str">
         <f>A11</f>
@@ -2152,7 +2147,7 @@
     </row>
     <row r="6" spans="1:30">
       <c r="A6" s="28" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C6" s="29" t="str">
         <f>C5</f>
@@ -2269,7 +2264,7 @@
     </row>
     <row r="7" spans="1:30">
       <c r="A7" s="28" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C7" s="29" t="str">
         <f>"*"&amp;C5</f>
@@ -2386,223 +2381,223 @@
     </row>
     <row r="10" spans="1:30" ht="15.75" thickBot="1">
       <c r="A10" s="31" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:30">
       <c r="A11" s="32" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:30">
       <c r="A12" s="33" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:30">
       <c r="A13" s="33" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B13" s="33" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:30">
       <c r="A14" s="33" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B14" s="33" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:30">
       <c r="A15" s="33" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B15" s="33" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:30">
       <c r="A16" s="33" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B16" s="33" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="33" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B17" s="33" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="33" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B18" s="33" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="33" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B19" s="33" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="33" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B20" s="33" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="33" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B21" s="33" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="33" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B22" s="33" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="33" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B23" s="33" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="33" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B24" s="33" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="33" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B25" s="33" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="33" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B26" s="33" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="33" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B27" s="33" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="33" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B28" s="33" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="33" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B29" s="33" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="33" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B30" s="33" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="33" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B31" s="33" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="33" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B32" s="33" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="33" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B33" s="33" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="33" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B34" s="33" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="33" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B35" s="33" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="33" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B36" s="33" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="34" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -2644,10 +2639,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B2:Q8"/>
+  <dimension ref="B2:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2655,10 +2650,10 @@
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="4" max="4" width="38.85546875" customWidth="1"/>
     <col min="5" max="5" width="20.5703125" customWidth="1"/>
-    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17">
+    <row r="2" spans="2:11">
       <c r="B2" s="10" t="s">
         <v>20</v>
       </c>
@@ -2671,14 +2666,8 @@
       <c r="I2" s="9"/>
       <c r="J2" s="11"/>
       <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-    </row>
-    <row r="3" spans="2:17" ht="15.75" thickBot="1">
+    </row>
+    <row r="3" spans="2:11" ht="15.75" thickBot="1">
       <c r="B3" s="13" t="s">
         <v>21</v>
       </c>
@@ -2711,31 +2700,13 @@
       <c r="K3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="M3" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="N3" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="O3" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="P3" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q3" s="15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="2:17">
+    </row>
+    <row r="4" spans="2:11">
       <c r="C4" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E4">
         <v>2050</v>
@@ -2751,15 +2722,15 @@
       </c>
       <c r="J4" s="17"/>
       <c r="K4" s="20" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="2:17">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11">
       <c r="C5" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E5">
         <v>2050</v>
@@ -2772,15 +2743,15 @@
         <v>8.7322500000000005</v>
       </c>
       <c r="K5" s="20" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="2:17">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11">
       <c r="C6" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E6">
         <v>2050</v>
@@ -2793,15 +2764,15 @@
         <v>5.7896999999999998</v>
       </c>
       <c r="K6" s="20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="2:17">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11">
       <c r="C7" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E7">
         <v>2050</v>
@@ -2814,28 +2785,149 @@
         <v>3.9777</v>
       </c>
       <c r="K7" s="20" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="2:17">
-      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11">
+      <c r="B8" s="35"/>
+      <c r="C8" s="35" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8">
+        <v>26</v>
+      </c>
+      <c r="E8" s="35">
         <v>2050</v>
       </c>
-      <c r="H8" s="16">
+      <c r="H8" s="35">
         <v>3.9907499999999998</v>
       </c>
-      <c r="I8" s="16">
+      <c r="I8" s="35">
         <f t="shared" si="0"/>
         <v>3.9907499999999998</v>
       </c>
-      <c r="K8" s="20" t="s">
-        <v>34</v>
+      <c r="K8" s="36" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11">
+      <c r="C9" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="28">
+        <v>0</v>
+      </c>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="28">
+        <v>3</v>
+      </c>
+      <c r="I9" s="28">
+        <f>H9</f>
+        <v>3</v>
+      </c>
+      <c r="J9" s="17"/>
+      <c r="K9" s="20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11">
+      <c r="C10" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="28">
+        <v>0</v>
+      </c>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28">
+        <v>3</v>
+      </c>
+      <c r="I10" s="28">
+        <f t="shared" ref="I10:I13" si="1">H10</f>
+        <v>3</v>
+      </c>
+      <c r="J10" s="28"/>
+      <c r="K10" s="20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11">
+      <c r="C11" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="28">
+        <v>0</v>
+      </c>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28">
+        <v>3</v>
+      </c>
+      <c r="I11" s="28">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="J11" s="28"/>
+      <c r="K11" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11">
+      <c r="C12" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="28">
+        <v>0</v>
+      </c>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28">
+        <v>3</v>
+      </c>
+      <c r="I12" s="28">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="J12" s="28"/>
+      <c r="K12" s="20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11">
+      <c r="C13" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="28">
+        <v>0</v>
+      </c>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28">
+        <v>3</v>
+      </c>
+      <c r="I13" s="28">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="J13" s="28"/>
+      <c r="K13" s="20" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -2848,18 +2940,18 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="B1:AC12"/>
+  <dimension ref="B1:W12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:29">
+    <row r="1" spans="2:23">
       <c r="B1" s="10" t="s">
         <v>20</v>
       </c>
@@ -2872,14 +2964,8 @@
       <c r="I1" s="16"/>
       <c r="J1" s="11"/>
       <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-    </row>
-    <row r="2" spans="2:29" ht="15.75" thickBot="1">
+    </row>
+    <row r="2" spans="2:23" ht="15.75" thickBot="1">
       <c r="B2" s="13" t="s">
         <v>21</v>
       </c>
@@ -2912,61 +2998,43 @@
       <c r="K2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="M2" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="N2" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="O2" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="P2" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q2" s="15" t="s">
-        <v>28</v>
+      <c r="N2" t="s">
+        <v>36</v>
+      </c>
+      <c r="O2" t="s">
+        <v>37</v>
+      </c>
+      <c r="P2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>39</v>
+      </c>
+      <c r="R2" t="s">
+        <v>40</v>
+      </c>
+      <c r="S2" t="s">
+        <v>41</v>
       </c>
       <c r="T2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="U2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="V2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="W2" t="s">
-        <v>42</v>
-      </c>
-      <c r="X2" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z2" t="s">
         <v>45</v>
       </c>
-      <c r="AA2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>47</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="2:29">
+    </row>
+    <row r="3" spans="2:23">
       <c r="C3" t="s">
         <v>14</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E3">
         <v>2020</v>
@@ -2982,45 +3050,45 @@
       </c>
       <c r="J3" s="17"/>
       <c r="K3" s="23" t="s">
-        <v>35</v>
+        <v>32</v>
+      </c>
+      <c r="N3" t="s">
+        <v>46</v>
+      </c>
+      <c r="O3" t="s">
+        <v>47</v>
+      </c>
+      <c r="P3" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>49</v>
+      </c>
+      <c r="R3">
+        <v>100</v>
+      </c>
+      <c r="S3" t="s">
+        <v>50</v>
       </c>
       <c r="T3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="U3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="V3" t="s">
-        <v>51</v>
-      </c>
-      <c r="W3" t="s">
-        <v>52</v>
-      </c>
-      <c r="X3">
-        <v>100</v>
-      </c>
-      <c r="Y3" t="s">
         <v>53</v>
       </c>
-      <c r="Z3" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>56</v>
-      </c>
-      <c r="AC3">
+      <c r="W3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:29">
+    <row r="4" spans="2:23">
       <c r="C4" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E4">
         <v>2025</v>
@@ -3033,45 +3101,45 @@
         <v>2.6998000000000002</v>
       </c>
       <c r="K4" s="23" t="s">
-        <v>35</v>
+        <v>32</v>
+      </c>
+      <c r="N4" t="s">
+        <v>46</v>
+      </c>
+      <c r="O4" t="s">
+        <v>47</v>
+      </c>
+      <c r="P4" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>49</v>
+      </c>
+      <c r="R4">
+        <v>100</v>
+      </c>
+      <c r="S4" t="s">
+        <v>50</v>
       </c>
       <c r="T4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="U4" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="V4" t="s">
-        <v>51</v>
-      </c>
-      <c r="W4" t="s">
-        <v>52</v>
-      </c>
-      <c r="X4">
-        <v>100</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>53</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>58</v>
-      </c>
-      <c r="AC4">
+        <v>55</v>
+      </c>
+      <c r="W4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:29">
+    <row r="5" spans="2:23">
       <c r="C5" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E5">
         <v>2030</v>
@@ -3084,45 +3152,45 @@
         <v>3.4620000000000002</v>
       </c>
       <c r="K5" s="23" t="s">
-        <v>35</v>
+        <v>32</v>
+      </c>
+      <c r="N5" t="s">
+        <v>46</v>
+      </c>
+      <c r="O5" t="s">
+        <v>47</v>
+      </c>
+      <c r="P5" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>56</v>
+      </c>
+      <c r="R5">
+        <v>100</v>
+      </c>
+      <c r="S5" t="s">
+        <v>50</v>
       </c>
       <c r="T5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="U5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="V5" t="s">
-        <v>51</v>
-      </c>
-      <c r="W5" t="s">
-        <v>59</v>
-      </c>
-      <c r="X5">
-        <v>100</v>
-      </c>
-      <c r="Y5" t="s">
         <v>53</v>
       </c>
-      <c r="Z5" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>56</v>
-      </c>
-      <c r="AC5">
+      <c r="W5">
         <v>0.75</v>
       </c>
     </row>
-    <row r="6" spans="2:29">
+    <row r="6" spans="2:23">
       <c r="C6" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E6">
         <v>2050</v>
@@ -3135,216 +3203,234 @@
         <v>3.4620000000000002</v>
       </c>
       <c r="K6" s="23" t="s">
-        <v>35</v>
+        <v>32</v>
+      </c>
+      <c r="N6" t="s">
+        <v>46</v>
+      </c>
+      <c r="O6" t="s">
+        <v>47</v>
+      </c>
+      <c r="P6" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>56</v>
+      </c>
+      <c r="R6">
+        <v>100</v>
+      </c>
+      <c r="S6" t="s">
+        <v>50</v>
       </c>
       <c r="T6" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="U6" t="s">
+        <v>54</v>
+      </c>
+      <c r="V6" t="s">
+        <v>55</v>
+      </c>
+      <c r="W6">
+        <v>3.4620000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="2:23">
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>5</v>
+      </c>
+      <c r="I7">
+        <v>5</v>
+      </c>
+      <c r="K7" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="N7" t="s">
+        <v>46</v>
+      </c>
+      <c r="O7" t="s">
+        <v>47</v>
+      </c>
+      <c r="P7" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>57</v>
+      </c>
+      <c r="R7">
+        <v>100</v>
+      </c>
+      <c r="S7" t="s">
         <v>50</v>
       </c>
-      <c r="V6" t="s">
+      <c r="T7" t="s">
         <v>51</v>
       </c>
-      <c r="W6" t="s">
+      <c r="U7" t="s">
+        <v>52</v>
+      </c>
+      <c r="V7" t="s">
+        <v>53</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:23">
+      <c r="N8" t="s">
+        <v>46</v>
+      </c>
+      <c r="O8" t="s">
+        <v>47</v>
+      </c>
+      <c r="P8" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>57</v>
+      </c>
+      <c r="R8">
+        <v>100</v>
+      </c>
+      <c r="S8" t="s">
+        <v>50</v>
+      </c>
+      <c r="T8" t="s">
+        <v>51</v>
+      </c>
+      <c r="U8" t="s">
+        <v>54</v>
+      </c>
+      <c r="V8" t="s">
+        <v>55</v>
+      </c>
+      <c r="W8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:23">
+      <c r="N9" t="s">
+        <v>46</v>
+      </c>
+      <c r="O9" t="s">
+        <v>58</v>
+      </c>
+      <c r="P9" t="s">
         <v>59</v>
       </c>
-      <c r="X6">
+      <c r="R9">
         <v>100</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="S9" t="s">
+        <v>50</v>
+      </c>
+      <c r="T9" t="s">
+        <v>51</v>
+      </c>
+      <c r="U9" t="s">
+        <v>52</v>
+      </c>
+      <c r="V9" t="s">
         <v>53</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="W9">
+        <v>35.200000000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="2:23">
+      <c r="N10" t="s">
+        <v>46</v>
+      </c>
+      <c r="O10" t="s">
+        <v>60</v>
+      </c>
+      <c r="P10" t="s">
+        <v>59</v>
+      </c>
+      <c r="R10">
+        <v>100</v>
+      </c>
+      <c r="S10" t="s">
+        <v>50</v>
+      </c>
+      <c r="T10" t="s">
+        <v>51</v>
+      </c>
+      <c r="U10" t="s">
+        <v>52</v>
+      </c>
+      <c r="V10" t="s">
+        <v>53</v>
+      </c>
+      <c r="W10">
+        <v>35.700000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="2:23">
+      <c r="N11" t="s">
+        <v>46</v>
+      </c>
+      <c r="O11" t="s">
+        <v>58</v>
+      </c>
+      <c r="P11" t="s">
+        <v>59</v>
+      </c>
+      <c r="R11">
+        <v>100</v>
+      </c>
+      <c r="S11" t="s">
+        <v>50</v>
+      </c>
+      <c r="T11" t="s">
+        <v>51</v>
+      </c>
+      <c r="U11" t="s">
         <v>54</v>
       </c>
-      <c r="AA6" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AC6">
-        <v>3.4620000000000002</v>
-      </c>
-    </row>
-    <row r="7" spans="2:29">
-      <c r="T7" t="s">
-        <v>49</v>
-      </c>
-      <c r="U7" t="s">
+      <c r="V11" t="s">
+        <v>55</v>
+      </c>
+      <c r="W11">
+        <v>137.4</v>
+      </c>
+    </row>
+    <row r="12" spans="2:23">
+      <c r="N12" t="s">
+        <v>46</v>
+      </c>
+      <c r="O12" t="s">
+        <v>60</v>
+      </c>
+      <c r="P12" t="s">
+        <v>59</v>
+      </c>
+      <c r="R12">
+        <v>100</v>
+      </c>
+      <c r="S12" t="s">
         <v>50</v>
       </c>
-      <c r="V7" t="s">
+      <c r="T12" t="s">
         <v>51</v>
       </c>
-      <c r="W7" t="s">
-        <v>60</v>
-      </c>
-      <c r="X7">
-        <v>100</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>53</v>
-      </c>
-      <c r="Z7" t="s">
+      <c r="U12" t="s">
         <v>54</v>
       </c>
-      <c r="AA7" t="s">
+      <c r="V12" t="s">
         <v>55</v>
       </c>
-      <c r="AB7" t="s">
-        <v>56</v>
-      </c>
-      <c r="AC7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:29">
-      <c r="T8" t="s">
-        <v>49</v>
-      </c>
-      <c r="U8" t="s">
-        <v>50</v>
-      </c>
-      <c r="V8" t="s">
-        <v>51</v>
-      </c>
-      <c r="W8" t="s">
-        <v>60</v>
-      </c>
-      <c r="X8">
-        <v>100</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>53</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>58</v>
-      </c>
-      <c r="AC8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:29">
-      <c r="T9" t="s">
-        <v>49</v>
-      </c>
-      <c r="U9" t="s">
-        <v>61</v>
-      </c>
-      <c r="V9" t="s">
-        <v>62</v>
-      </c>
-      <c r="X9">
-        <v>100</v>
-      </c>
-      <c r="Y9" t="s">
-        <v>53</v>
-      </c>
-      <c r="Z9" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA9" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB9" t="s">
-        <v>56</v>
-      </c>
-      <c r="AC9">
-        <v>35.200000000000003</v>
-      </c>
-    </row>
-    <row r="10" spans="2:29">
-      <c r="T10" t="s">
-        <v>49</v>
-      </c>
-      <c r="U10" t="s">
-        <v>63</v>
-      </c>
-      <c r="V10" t="s">
-        <v>62</v>
-      </c>
-      <c r="X10">
-        <v>100</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>53</v>
-      </c>
-      <c r="Z10" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA10" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB10" t="s">
-        <v>56</v>
-      </c>
-      <c r="AC10">
-        <v>35.700000000000003</v>
-      </c>
-    </row>
-    <row r="11" spans="2:29">
-      <c r="T11" t="s">
-        <v>49</v>
-      </c>
-      <c r="U11" t="s">
-        <v>61</v>
-      </c>
-      <c r="V11" t="s">
-        <v>62</v>
-      </c>
-      <c r="X11">
-        <v>100</v>
-      </c>
-      <c r="Y11" t="s">
-        <v>53</v>
-      </c>
-      <c r="Z11" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA11" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB11" t="s">
-        <v>58</v>
-      </c>
-      <c r="AC11">
-        <v>137.4</v>
-      </c>
-    </row>
-    <row r="12" spans="2:29">
-      <c r="T12" t="s">
-        <v>49</v>
-      </c>
-      <c r="U12" t="s">
-        <v>63</v>
-      </c>
-      <c r="V12" t="s">
-        <v>62</v>
-      </c>
-      <c r="X12">
-        <v>100</v>
-      </c>
-      <c r="Y12" t="s">
-        <v>53</v>
-      </c>
-      <c r="Z12" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA12" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB12" t="s">
-        <v>58</v>
-      </c>
-      <c r="AC12">
+      <c r="W12">
         <v>139.9</v>
       </c>
     </row>
@@ -3358,19 +3444,19 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="B3:S14"/>
+  <dimension ref="B3:M15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="44.42578125" customWidth="1"/>
-    <col min="11" max="11" width="54.140625" customWidth="1"/>
+    <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:19">
+    <row r="3" spans="2:13">
       <c r="B3" s="10" t="s">
         <v>20</v>
       </c>
@@ -3383,14 +3469,8 @@
       <c r="I3" s="16"/>
       <c r="J3" s="11"/>
       <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="12"/>
-    </row>
-    <row r="4" spans="2:19" ht="15.75" thickBot="1">
+    </row>
+    <row r="4" spans="2:13" ht="15.75" thickBot="1">
       <c r="B4" s="13" t="s">
         <v>21</v>
       </c>
@@ -3423,32 +3503,14 @@
       <c r="K4" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="L4" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="M4" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="N4" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="O4" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="P4" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q4" s="15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="2:19">
+    </row>
+    <row r="5" spans="2:13">
       <c r="B5" s="16"/>
       <c r="C5" s="16" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E5" s="16">
         <v>2030</v>
@@ -3464,22 +3526,16 @@
       </c>
       <c r="J5" s="16"/>
       <c r="K5" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="L5" s="16"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="16"/>
-      <c r="P5" s="16"/>
-      <c r="Q5" s="16"/>
-    </row>
-    <row r="6" spans="2:19">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13">
       <c r="B6" s="16"/>
       <c r="C6" s="16" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E6" s="16">
         <v>2040</v>
@@ -3495,21 +3551,15 @@
       </c>
       <c r="J6" s="16"/>
       <c r="K6" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="16"/>
-      <c r="O6" s="16"/>
-      <c r="P6" s="16"/>
-      <c r="Q6" s="16"/>
-    </row>
-    <row r="7" spans="2:19">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13">
       <c r="C7" s="16" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E7" s="16">
         <v>2050</v>
@@ -3522,179 +3572,180 @@
         <v>31.1</v>
       </c>
       <c r="K7" s="22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="2:19">
-      <c r="B9" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" s="28" customFormat="1">
+      <c r="C8" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="28">
+        <v>0</v>
+      </c>
+      <c r="H8" s="28">
+        <v>5</v>
+      </c>
+      <c r="I8" s="28">
+        <f t="shared" ref="I8" si="1">H8</f>
+        <v>5</v>
+      </c>
+      <c r="K8" s="22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13">
+      <c r="B10" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="12"/>
-      <c r="Q9" s="12"/>
-    </row>
-    <row r="10" spans="2:19" ht="15.75" thickBot="1">
-      <c r="B10" s="13" t="s">
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="12"/>
+    </row>
+    <row r="11" spans="2:13" ht="15.75" thickBot="1">
+      <c r="B11" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C11" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D11" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E11" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F11" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="G11" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="H10" s="14" t="str">
+      <c r="H11" s="14" t="str">
         <f>Regions!C3</f>
         <v>IE</v>
       </c>
-      <c r="I10" s="14" t="str">
+      <c r="I11" s="14" t="str">
         <f>Regions!D3</f>
         <v>National</v>
       </c>
-      <c r="J10" s="15" t="s">
+      <c r="J11" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="K10" s="15" t="s">
+      <c r="K11" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="L10" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="M10" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="N10" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="O10" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="P10" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q10" s="15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="2:19">
-      <c r="B11" s="16"/>
-      <c r="C11" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="16">
-        <v>2030</v>
-      </c>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16">
-        <v>0.25</v>
-      </c>
-      <c r="I11">
-        <f>H11</f>
-        <v>0.25</v>
-      </c>
-      <c r="J11" s="16"/>
-      <c r="K11" s="22" t="s">
-        <v>96</v>
-      </c>
-      <c r="L11" s="16"/>
-      <c r="M11" s="16"/>
-      <c r="N11" s="16"/>
-      <c r="O11" s="16"/>
-      <c r="P11" s="16"/>
-      <c r="Q11" s="16"/>
-    </row>
-    <row r="12" spans="2:19">
+    </row>
+    <row r="12" spans="2:13">
       <c r="B12" s="16"/>
       <c r="C12" s="16" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E12" s="16">
-        <v>2040</v>
+        <v>2030</v>
       </c>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
       <c r="H12" s="16">
-        <v>0.5</v>
-      </c>
-      <c r="I12" s="16">
-        <f t="shared" ref="I12:I13" si="1">H12</f>
-        <v>0.5</v>
+        <v>0.25</v>
+      </c>
+      <c r="I12">
+        <f>H12</f>
+        <v>0.25</v>
       </c>
       <c r="J12" s="16"/>
       <c r="K12" s="22" t="s">
-        <v>96</v>
-      </c>
-      <c r="L12" s="16"/>
-      <c r="M12" s="16"/>
-      <c r="N12" s="16"/>
-      <c r="O12" s="16"/>
-      <c r="P12" s="16"/>
-      <c r="Q12" s="16"/>
-    </row>
-    <row r="13" spans="2:19">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13">
       <c r="B13" s="16"/>
       <c r="C13" s="16" t="s">
         <v>14</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E13" s="16">
-        <v>2050</v>
+        <v>2040</v>
       </c>
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
-      <c r="H13">
-        <v>1</v>
+      <c r="H13" s="16">
+        <v>0.5</v>
       </c>
       <c r="I13" s="16">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f t="shared" ref="I13:I14" si="2">H13</f>
+        <v>0.5</v>
       </c>
       <c r="J13" s="16"/>
       <c r="K13" s="22" t="s">
-        <v>96</v>
-      </c>
-      <c r="L13" s="16"/>
-      <c r="M13" s="16"/>
-      <c r="N13" s="16"/>
-      <c r="O13" s="16"/>
-      <c r="P13" s="16"/>
-      <c r="Q13" s="16"/>
-      <c r="S13" s="24" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="14" spans="2:19">
-      <c r="S14" s="16">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13">
+      <c r="B14" s="16"/>
+      <c r="C14" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="16">
+        <v>2050</v>
+      </c>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14" s="16">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J14" s="16"/>
+      <c r="K14" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="M14" s="24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13">
+      <c r="C15" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="28">
+        <v>0</v>
+      </c>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28">
+        <v>5</v>
+      </c>
+      <c r="I15" s="28">
+        <f t="shared" ref="I15" si="3">H15</f>
+        <v>5</v>
+      </c>
+      <c r="J15" s="28"/>
+      <c r="K15" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="M15" s="16">
         <f>2.63*1000/8760/0.3</f>
         <v>1.0007610350076104</v>
       </c>
@@ -3712,14 +3763,18 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:V48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="15.140625" customWidth="1"/>
     <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="28.28515625" customWidth="1"/>
     <col min="20" max="20" width="27.7109375" customWidth="1"/>
   </cols>
@@ -3740,7 +3795,7 @@
         <v>10</v>
       </c>
       <c r="S3" s="25" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:22">
@@ -3748,7 +3803,7 @@
         <v>7</v>
       </c>
       <c r="S4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="U4" s="26">
         <v>0.12</v>
@@ -3798,7 +3853,7 @@
         <v>11</v>
       </c>
       <c r="S5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:22">
@@ -3806,10 +3861,10 @@
         <v>15</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G6" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I6">
         <v>2020</v>
@@ -3830,21 +3885,18 @@
         <v>17</v>
       </c>
       <c r="U6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="V6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:22">
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
       <c r="D7" s="21" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G7" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I7">
         <v>2050</v>
@@ -3860,24 +3912,24 @@
       </c>
       <c r="M7" s="3"/>
       <c r="S7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="T7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="U7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="V7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:22">
       <c r="S8" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="T8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="U8">
         <v>10127</v>
@@ -3888,10 +3940,10 @@
     </row>
     <row r="9" spans="1:22">
       <c r="S9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="T9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="U9">
         <v>83</v>
@@ -3902,10 +3954,10 @@
     </row>
     <row r="10" spans="1:22">
       <c r="S10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="T10" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="U10">
         <v>56</v>
@@ -3934,10 +3986,10 @@
       <c r="P11" s="12"/>
       <c r="Q11" s="12"/>
       <c r="S11" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="T11" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="U11">
         <v>56</v>
@@ -3974,29 +4026,11 @@
       <c r="J12" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="K12" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="L12" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="M12" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="N12" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="O12" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="P12" s="15" t="s">
-        <v>28</v>
-      </c>
       <c r="S12" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="T12" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="U12">
         <v>87</v>
@@ -4011,7 +4045,7 @@
         <v>14</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E13" s="16">
         <v>2050</v>
@@ -4023,7 +4057,7 @@
       </c>
       <c r="I13" s="17"/>
       <c r="J13" s="27" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="K13" s="16"/>
       <c r="L13" s="16"/>
@@ -4032,10 +4066,10 @@
       <c r="O13" s="16"/>
       <c r="P13" s="16"/>
       <c r="S13" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="T13" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="U13">
         <v>108</v>
@@ -4062,10 +4096,10 @@
       <c r="P14" s="16"/>
       <c r="Q14" s="16"/>
       <c r="S14" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="T14" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="U14">
         <v>108</v>
@@ -4092,10 +4126,10 @@
       <c r="P15" s="16"/>
       <c r="Q15" s="16"/>
       <c r="S15" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="T15" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="U15">
         <v>108</v>
@@ -4122,10 +4156,10 @@
       <c r="P16" s="16"/>
       <c r="Q16" s="16"/>
       <c r="S16" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="T16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="U16">
         <v>37</v>
@@ -4152,10 +4186,10 @@
       <c r="P17" s="16"/>
       <c r="Q17" s="16"/>
       <c r="S17" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="T17" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="U17">
         <v>25</v>
@@ -4166,10 +4200,10 @@
     </row>
     <row r="18" spans="2:22">
       <c r="S18" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="T18" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="U18">
         <v>25</v>
@@ -4180,10 +4214,10 @@
     </row>
     <row r="19" spans="2:22">
       <c r="S19" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="T19" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="U19">
         <v>287</v>
@@ -4194,10 +4228,10 @@
     </row>
     <row r="20" spans="2:22">
       <c r="S20" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="T20" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="U20">
         <v>66</v>
@@ -4208,10 +4242,10 @@
     </row>
     <row r="21" spans="2:22">
       <c r="S21" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="T21" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="U21">
         <v>66</v>
@@ -4222,10 +4256,10 @@
     </row>
     <row r="22" spans="2:22">
       <c r="S22" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="T22" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="U22">
         <v>66</v>
@@ -4236,10 +4270,10 @@
     </row>
     <row r="23" spans="2:22">
       <c r="S23" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="T23" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="U23">
         <v>598</v>
@@ -4250,10 +4284,10 @@
     </row>
     <row r="24" spans="2:22">
       <c r="S24" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="T24" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="U24">
         <v>7867</v>
@@ -4264,10 +4298,10 @@
     </row>
     <row r="25" spans="2:22">
       <c r="S25" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="T25" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="U25">
         <v>26</v>
@@ -4278,10 +4312,10 @@
     </row>
     <row r="26" spans="2:22">
       <c r="S26" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="T26" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="U26">
         <v>458</v>
@@ -4292,32 +4326,32 @@
     </row>
     <row r="28" spans="2:22">
       <c r="U28" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="V28" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="2:22">
       <c r="S29" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="T29" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="U29" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="V29" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="2:22">
       <c r="S30" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="T30" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="U30">
         <v>10663</v>
@@ -4328,10 +4362,10 @@
     </row>
     <row r="31" spans="2:22">
       <c r="S31" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="T31" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="U31">
         <v>84</v>
@@ -4342,10 +4376,10 @@
     </row>
     <row r="32" spans="2:22">
       <c r="S32" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="T32" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="U32">
         <v>56</v>
@@ -4356,10 +4390,10 @@
     </row>
     <row r="33" spans="19:22">
       <c r="S33" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="T33" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="U33">
         <v>56</v>
@@ -4370,10 +4404,10 @@
     </row>
     <row r="34" spans="19:22">
       <c r="S34" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="T34" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="U34">
         <v>92</v>
@@ -4384,10 +4418,10 @@
     </row>
     <row r="35" spans="19:22">
       <c r="S35" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="T35" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="U35">
         <v>110</v>
@@ -4398,10 +4432,10 @@
     </row>
     <row r="36" spans="19:22">
       <c r="S36" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="T36" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="U36">
         <v>110</v>
@@ -4412,10 +4446,10 @@
     </row>
     <row r="37" spans="19:22">
       <c r="S37" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="T37" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="U37">
         <v>110</v>
@@ -4426,10 +4460,10 @@
     </row>
     <row r="38" spans="19:22">
       <c r="S38" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="T38" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="U38">
         <v>37</v>
@@ -4440,10 +4474,10 @@
     </row>
     <row r="39" spans="19:22">
       <c r="S39" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="T39" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="U39">
         <v>25</v>
@@ -4454,10 +4488,10 @@
     </row>
     <row r="40" spans="19:22">
       <c r="S40" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="T40" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="U40">
         <v>25</v>
@@ -4468,10 +4502,10 @@
     </row>
     <row r="41" spans="19:22">
       <c r="S41" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="T41" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="U41">
         <v>291</v>
@@ -4482,10 +4516,10 @@
     </row>
     <row r="42" spans="19:22">
       <c r="S42" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="T42" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="U42">
         <v>68</v>
@@ -4496,10 +4530,10 @@
     </row>
     <row r="43" spans="19:22">
       <c r="S43" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="T43" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="U43">
         <v>68</v>
@@ -4510,10 +4544,10 @@
     </row>
     <row r="44" spans="19:22">
       <c r="S44" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="T44" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="U44">
         <v>68</v>
@@ -4524,10 +4558,10 @@
     </row>
     <row r="45" spans="19:22">
       <c r="S45" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="T45" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="U45">
         <v>743</v>
@@ -4538,10 +4572,10 @@
     </row>
     <row r="46" spans="19:22">
       <c r="S46" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="T46" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="U46">
         <v>8175</v>
@@ -4552,10 +4586,10 @@
     </row>
     <row r="47" spans="19:22">
       <c r="S47" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="T47" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="U47">
         <v>34</v>
@@ -4566,10 +4600,10 @@
     </row>
     <row r="48" spans="19:22">
       <c r="S48" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="T48" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="U48">
         <v>511</v>
@@ -4590,14 +4624,17 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
     <col min="11" max="11" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -4667,10 +4704,10 @@
         <v>18</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G6" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I6">
         <v>2020</v>
@@ -4688,18 +4725,15 @@
         <v>15</v>
       </c>
       <c r="N6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:14">
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
       <c r="D7" s="21" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G7" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I7">
         <v>2050</v>

</xml_diff>

<commit_message>
added 2 new constraints (WON, WOF) to enable socially acceptable wind potentials on top of existing technical onshore and offshore potentials
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_PWR_RNW_Potentials.xlsx
+++ b/SuppXLS/Scen_PWR_RNW_Potentials.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_TIM\main\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B3AC272-34A3-4536-99FD-6EEB4D3FA7B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EACFA93C-A90C-4741-A842-B085EF1D6549}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4050" yWindow="3120" windowWidth="42510" windowHeight="23985" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="6" r:id="rId1"/>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="163">
   <si>
     <t>UC_N</t>
   </si>
@@ -568,6 +568,27 @@
   </si>
   <si>
     <t>ELCC</t>
+  </si>
+  <si>
+    <t>P-RNW-WIN-ON0*</t>
+  </si>
+  <si>
+    <t>UC_CAP</t>
+  </si>
+  <si>
+    <t>ELC_WONCAP</t>
+  </si>
+  <si>
+    <t>ELC_WOFCAP</t>
+  </si>
+  <si>
+    <t>P-RNW-WIN-OF0*</t>
+  </si>
+  <si>
+    <t>WIND_OFFSHORE_Socialy_Acceptable_Potential</t>
+  </si>
+  <si>
+    <t>WIND_ONSHORE_Socialy_Acceptable_Potential</t>
   </si>
 </sst>
 </file>
@@ -2639,10 +2660,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B2:K13"/>
+  <dimension ref="A2:N23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O25" sqref="O25"/>
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2651,6 +2672,7 @@
     <col min="4" max="4" width="38.85546875" customWidth="1"/>
     <col min="5" max="5" width="20.5703125" customWidth="1"/>
     <col min="11" max="11" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:11">
@@ -2929,6 +2951,183 @@
       <c r="K13" s="20" t="s">
         <v>31</v>
       </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="28"/>
+      <c r="N17" s="28"/>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="28"/>
+      <c r="B18" s="1" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,"~UC_Sets: R_E:",_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,"")))</f>
+        <v>~UC_Sets: R_E: IE,National</v>
+      </c>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="28"/>
+      <c r="N18" s="28"/>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="28"/>
+      <c r="B19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="28"/>
+      <c r="L19" s="28"/>
+      <c r="M19" s="28"/>
+      <c r="N19" s="28"/>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="28"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="K20" s="28"/>
+      <c r="L20" s="28"/>
+      <c r="M20" s="28"/>
+      <c r="N20" s="28"/>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="28"/>
+      <c r="B21" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="L21" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M21" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N21" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="28"/>
+      <c r="B22" s="28" t="s">
+        <v>158</v>
+      </c>
+      <c r="C22" s="28"/>
+      <c r="D22" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="E22" s="28"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="H22" s="28"/>
+      <c r="I22" s="28">
+        <v>2020</v>
+      </c>
+      <c r="J22" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="K22" s="28">
+        <v>1</v>
+      </c>
+      <c r="L22" s="28">
+        <v>5.72</v>
+      </c>
+      <c r="M22" s="28">
+        <v>15</v>
+      </c>
+      <c r="N22" s="28" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="28"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="H23" s="28"/>
+      <c r="I23" s="28">
+        <v>2050</v>
+      </c>
+      <c r="J23" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="K23" s="28">
+        <v>1</v>
+      </c>
+      <c r="L23" s="28">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="M23" s="3"/>
+      <c r="N23" s="28"/>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
@@ -2940,10 +3139,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="B1:W12"/>
+  <dimension ref="A1:W21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2951,7 +3150,7 @@
     <col min="11" max="11" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:23">
+    <row r="1" spans="1:23">
       <c r="B1" s="10" t="s">
         <v>20</v>
       </c>
@@ -2965,7 +3164,7 @@
       <c r="J1" s="11"/>
       <c r="K1" s="12"/>
     </row>
-    <row r="2" spans="2:23" ht="15.75" thickBot="1">
+    <row r="2" spans="1:23" ht="15.75" thickBot="1">
       <c r="B2" s="13" t="s">
         <v>21</v>
       </c>
@@ -3029,7 +3228,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="2:23">
+    <row r="3" spans="1:23">
       <c r="C3" t="s">
         <v>14</v>
       </c>
@@ -3083,7 +3282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:23">
+    <row r="4" spans="1:23">
       <c r="C4" t="s">
         <v>14</v>
       </c>
@@ -3134,7 +3333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:23">
+    <row r="5" spans="1:23">
       <c r="C5" t="s">
         <v>14</v>
       </c>
@@ -3185,7 +3384,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="6" spans="2:23">
+    <row r="6" spans="1:23">
       <c r="C6" t="s">
         <v>14</v>
       </c>
@@ -3236,7 +3435,7 @@
         <v>3.4620000000000002</v>
       </c>
     </row>
-    <row r="7" spans="2:23">
+    <row r="7" spans="1:23">
       <c r="C7" t="s">
         <v>14</v>
       </c>
@@ -3286,7 +3485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:23">
+    <row r="8" spans="1:23">
       <c r="N8" t="s">
         <v>46</v>
       </c>
@@ -3318,7 +3517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:23">
+    <row r="9" spans="1:23">
       <c r="N9" t="s">
         <v>46</v>
       </c>
@@ -3347,7 +3546,7 @@
         <v>35.200000000000003</v>
       </c>
     </row>
-    <row r="10" spans="2:23">
+    <row r="10" spans="1:23">
       <c r="N10" t="s">
         <v>46</v>
       </c>
@@ -3376,7 +3575,7 @@
         <v>35.700000000000003</v>
       </c>
     </row>
-    <row r="11" spans="2:23">
+    <row r="11" spans="1:23">
       <c r="N11" t="s">
         <v>46</v>
       </c>
@@ -3405,7 +3604,7 @@
         <v>137.4</v>
       </c>
     </row>
-    <row r="12" spans="2:23">
+    <row r="12" spans="1:23">
       <c r="N12" t="s">
         <v>46</v>
       </c>
@@ -3433,6 +3632,204 @@
       <c r="W12">
         <v>139.9</v>
       </c>
+    </row>
+    <row r="15" spans="1:23">
+      <c r="A15" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="28"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="28"/>
+      <c r="N15" s="28"/>
+      <c r="O15" s="28"/>
+      <c r="P15" s="28"/>
+      <c r="Q15" s="28"/>
+    </row>
+    <row r="16" spans="1:23">
+      <c r="A16" s="28"/>
+      <c r="B16" s="1" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,"~UC_Sets: R_E:",_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,"")))</f>
+        <v>~UC_Sets: R_E: IE,National</v>
+      </c>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="28"/>
+      <c r="N16" s="28"/>
+      <c r="O16" s="28"/>
+      <c r="P16" s="28"/>
+      <c r="Q16" s="28"/>
+    </row>
+    <row r="17" spans="1:17">
+      <c r="A17" s="28"/>
+      <c r="B17" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="28"/>
+      <c r="N17" s="28"/>
+      <c r="O17" s="28"/>
+      <c r="P17" s="28"/>
+      <c r="Q17" s="28"/>
+    </row>
+    <row r="18" spans="1:17">
+      <c r="A18" s="28"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="K18" s="28"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="28"/>
+      <c r="N18" s="28"/>
+      <c r="O18" s="28"/>
+      <c r="P18" s="28"/>
+      <c r="Q18" s="28"/>
+    </row>
+    <row r="19" spans="1:17">
+      <c r="A19" s="28"/>
+      <c r="B19" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N19" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="O19" s="28"/>
+      <c r="P19" s="28"/>
+      <c r="Q19" s="28"/>
+    </row>
+    <row r="20" spans="1:17">
+      <c r="A20" s="28"/>
+      <c r="B20" s="28" t="s">
+        <v>159</v>
+      </c>
+      <c r="C20" s="28"/>
+      <c r="D20" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="H20" s="28"/>
+      <c r="I20" s="28">
+        <v>2020</v>
+      </c>
+      <c r="J20" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="K20" s="28">
+        <v>1</v>
+      </c>
+      <c r="L20" s="28">
+        <v>1.03</v>
+      </c>
+      <c r="M20" s="28">
+        <v>15</v>
+      </c>
+      <c r="N20" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="O20" s="28"/>
+      <c r="P20" s="28"/>
+      <c r="Q20" s="28"/>
+    </row>
+    <row r="21" spans="1:17">
+      <c r="A21" s="28"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="H21" s="28"/>
+      <c r="I21" s="28">
+        <v>2050</v>
+      </c>
+      <c r="J21" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="K21" s="28">
+        <v>1</v>
+      </c>
+      <c r="L21" s="28">
+        <v>7.5</v>
+      </c>
+      <c r="M21" s="3"/>
+      <c r="N21" s="28"/>
+      <c r="O21" s="28"/>
+      <c r="P21" s="28"/>
+      <c r="Q21" s="28"/>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
@@ -3763,8 +4160,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:V48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Updating the upper bounds of growth rates of wind onshore and offshore
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_PWR_RNW_Potentials.xlsx
+++ b/SuppXLS/Scen_PWR_RNW_Potentials.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_TIM\main\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_TIM\main-40\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EACFA93C-A90C-4741-A842-B085EF1D6549}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF69CAF-1F32-4EB3-98F5-DFF8E253F98E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4050" yWindow="3120" windowWidth="42510" windowHeight="23985" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-34410" yWindow="-9135" windowWidth="28110" windowHeight="15885" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="6" r:id="rId1"/>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="165">
   <si>
     <t>UC_N</t>
   </si>
@@ -178,15 +178,15 @@
   </si>
   <si>
     <t>P-RNW-SOL*</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>P-RNW-HYD*</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>P-RNW-OCE-WAV01</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Country</t>
@@ -362,11 +362,11 @@
   </si>
   <si>
     <t>P-RNW-OCE-TID02</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>P-RNW-SOL-CSP04</t>
     <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>P-RNW-SOL-CSP04</t>
-    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Development</t>
@@ -576,31 +576,44 @@
     <t>UC_CAP</t>
   </si>
   <si>
-    <t>ELC_WONCAP</t>
-  </si>
-  <si>
-    <t>ELC_WOFCAP</t>
-  </si>
-  <si>
     <t>P-RNW-WIN-OF0*</t>
   </si>
   <si>
     <t>WIND_OFFSHORE_Socialy_Acceptable_Potential</t>
   </si>
   <si>
-    <t>WIND_ONSHORE_Socialy_Acceptable_Potential</t>
+    <t>UC_NCAP</t>
+  </si>
+  <si>
+    <t>PWR_WONCAP</t>
+  </si>
+  <si>
+    <t>PWR_WONNCAP</t>
+  </si>
+  <si>
+    <t>PWR_WOFCAP</t>
+  </si>
+  <si>
+    <t>PWR_WOFNCAP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="30">
+  <fonts count="31">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1221,147 +1234,147 @@
   </borders>
   <cellStyleXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1369,30 +1382,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="29" fillId="36" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="36" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="36" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="30" fillId="36" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="37" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="37" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
@@ -1400,6 +1413,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="40">
     <cellStyle name="20% - Accent1" xfId="17" builtinId="30" customBuiltin="1"/>
@@ -2660,10 +2674,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A2:N23"/>
+  <dimension ref="A2:N68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2672,10 +2686,11 @@
     <col min="4" max="4" width="38.85546875" customWidth="1"/>
     <col min="5" max="5" width="20.5703125" customWidth="1"/>
     <col min="11" max="11" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11">
+    <row r="2" spans="1:14">
       <c r="B2" s="10" t="s">
         <v>20</v>
       </c>
@@ -2689,7 +2704,7 @@
       <c r="J2" s="11"/>
       <c r="K2" s="12"/>
     </row>
-    <row r="3" spans="2:11" ht="15.75" thickBot="1">
+    <row r="3" spans="1:14" ht="15.75" thickBot="1">
       <c r="B3" s="13" t="s">
         <v>21</v>
       </c>
@@ -2723,7 +2738,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:11">
+    <row r="4" spans="1:14">
       <c r="C4" t="s">
         <v>14</v>
       </c>
@@ -2747,7 +2762,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="2:11">
+    <row r="5" spans="1:14">
       <c r="C5" t="s">
         <v>14</v>
       </c>
@@ -2768,7 +2783,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="2:11">
+    <row r="6" spans="1:14">
       <c r="C6" t="s">
         <v>14</v>
       </c>
@@ -2789,7 +2804,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="2:11">
+    <row r="7" spans="1:14">
       <c r="C7" t="s">
         <v>14</v>
       </c>
@@ -2810,7 +2825,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="2:11">
+    <row r="8" spans="1:14">
       <c r="B8" s="35"/>
       <c r="C8" s="35" t="s">
         <v>14</v>
@@ -2832,7 +2847,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="2:11">
+    <row r="9" spans="1:14">
       <c r="C9" s="28" t="s">
         <v>14</v>
       </c>
@@ -2856,7 +2871,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="2:11">
+    <row r="10" spans="1:14">
       <c r="C10" s="28" t="s">
         <v>14</v>
       </c>
@@ -2880,7 +2895,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="2:11">
+    <row r="11" spans="1:14">
       <c r="C11" s="28" t="s">
         <v>14</v>
       </c>
@@ -2904,7 +2919,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="2:11">
+    <row r="12" spans="1:14">
       <c r="C12" s="28" t="s">
         <v>14</v>
       </c>
@@ -2928,7 +2943,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="2:11">
+    <row r="13" spans="1:14">
       <c r="C13" s="28" t="s">
         <v>14</v>
       </c>
@@ -2952,11 +2967,48 @@
         <v>31</v>
       </c>
     </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="28"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="28"/>
+      <c r="N15" s="28"/>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="28"/>
+      <c r="B16" s="1" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,"~UC_Sets: R_E:",_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,"")))</f>
+        <v>~UC_Sets: R_E: IE,National</v>
+      </c>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="28"/>
+      <c r="N16" s="28"/>
+    </row>
     <row r="17" spans="1:14">
-      <c r="A17" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" s="28"/>
+      <c r="A17" s="28"/>
+      <c r="B17" s="6" t="s">
+        <v>10</v>
+      </c>
       <c r="C17" s="28"/>
       <c r="D17" s="28"/>
       <c r="E17" s="28"/>
@@ -2972,10 +3024,7 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="28"/>
-      <c r="B18" s="1" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,"~UC_Sets: R_E:",_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,"")))</f>
-        <v>~UC_Sets: R_E: IE,National</v>
-      </c>
+      <c r="B18" s="28"/>
       <c r="C18" s="28"/>
       <c r="D18" s="28"/>
       <c r="E18" s="28"/>
@@ -2983,7 +3032,9 @@
       <c r="G18" s="28"/>
       <c r="H18" s="28"/>
       <c r="I18" s="28"/>
-      <c r="J18" s="28"/>
+      <c r="J18" s="28" t="s">
+        <v>7</v>
+      </c>
       <c r="K18" s="28"/>
       <c r="L18" s="28"/>
       <c r="M18" s="28"/>
@@ -2991,99 +3042,111 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="28"/>
-      <c r="B19" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
-      <c r="K19" s="28"/>
-      <c r="L19" s="28"/>
-      <c r="M19" s="28"/>
-      <c r="N19" s="28"/>
+      <c r="B19" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M19" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="28"/>
-      <c r="B20" s="28"/>
+      <c r="B20" s="37" t="s">
+        <v>161</v>
+      </c>
       <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
+      <c r="D20" s="20" t="s">
+        <v>156</v>
+      </c>
       <c r="E20" s="28"/>
       <c r="F20" s="28"/>
-      <c r="G20" s="28"/>
+      <c r="G20" s="28" t="s">
+        <v>155</v>
+      </c>
       <c r="H20" s="28"/>
-      <c r="I20" s="28"/>
+      <c r="I20" s="28">
+        <v>2019</v>
+      </c>
       <c r="J20" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="K20" s="28"/>
-      <c r="L20" s="28"/>
-      <c r="M20" s="28"/>
-      <c r="N20" s="28"/>
+        <v>14</v>
+      </c>
+      <c r="K20" s="28">
+        <v>1</v>
+      </c>
+      <c r="L20" s="28">
+        <v>4</v>
+      </c>
+      <c r="M20" s="28">
+        <v>5</v>
+      </c>
     </row>
     <row r="21" spans="1:14">
       <c r="A21" s="28"/>
-      <c r="B21" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="2" t="s">
+      <c r="B21" s="28"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="H21" s="28"/>
+      <c r="I21" s="28">
+        <v>2020</v>
+      </c>
+      <c r="J21" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="K21" s="28">
         <v>1</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H21" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I21" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="J21" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="K21" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="L21" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="M21" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="N21" s="7" t="s">
-        <v>11</v>
-      </c>
+      <c r="L21" s="28">
+        <v>5.2</v>
+      </c>
+      <c r="M21" s="28"/>
     </row>
     <row r="22" spans="1:14">
-      <c r="A22" s="28"/>
-      <c r="B22" s="28" t="s">
-        <v>158</v>
-      </c>
-      <c r="C22" s="28"/>
       <c r="D22" s="20" t="s">
         <v>156</v>
       </c>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
       <c r="G22" s="28" t="s">
         <v>155</v>
       </c>
       <c r="H22" s="28"/>
       <c r="I22" s="28">
-        <v>2020</v>
+        <v>2025</v>
       </c>
       <c r="J22" s="28" t="s">
         <v>14</v>
@@ -3092,30 +3155,19 @@
         <v>1</v>
       </c>
       <c r="L22" s="28">
-        <v>5.72</v>
-      </c>
-      <c r="M22" s="28">
-        <v>15</v>
-      </c>
-      <c r="N22" s="28" t="s">
-        <v>162</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="23" spans="1:14">
-      <c r="A23" s="28"/>
-      <c r="B23" s="28"/>
-      <c r="C23" s="28"/>
       <c r="D23" s="20" t="s">
         <v>156</v>
       </c>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
       <c r="G23" s="28" t="s">
         <v>155</v>
       </c>
       <c r="H23" s="28"/>
       <c r="I23" s="28">
-        <v>2050</v>
+        <v>2030</v>
       </c>
       <c r="J23" s="28" t="s">
         <v>14</v>
@@ -3124,13 +3176,323 @@
         <v>1</v>
       </c>
       <c r="L23" s="28">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="M23" s="3"/>
-      <c r="N23" s="28"/>
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="D24" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="G24" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="H24" s="28"/>
+      <c r="I24" s="28">
+        <v>2050</v>
+      </c>
+      <c r="J24" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="K24" s="28">
+        <v>1</v>
+      </c>
+      <c r="L24" s="28">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="A30" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" s="28"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="28"/>
+      <c r="I30" s="28"/>
+      <c r="J30" s="28"/>
+      <c r="K30" s="28"/>
+      <c r="M30" s="28"/>
+      <c r="N30" s="28"/>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31" s="28"/>
+      <c r="B31" s="1" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,"~UC_Sets: R_E:",_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,"")))</f>
+        <v>~UC_Sets: R_E: IE,National</v>
+      </c>
+      <c r="C31" s="28"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="28"/>
+      <c r="H31" s="28"/>
+      <c r="I31" s="28"/>
+      <c r="J31" s="28"/>
+      <c r="K31" s="28"/>
+      <c r="M31" s="28"/>
+      <c r="N31" s="28"/>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32" s="28"/>
+      <c r="B32" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" s="28"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="28"/>
+      <c r="H32" s="28"/>
+      <c r="I32" s="28"/>
+      <c r="J32" s="28"/>
+      <c r="K32" s="28"/>
+      <c r="M32" s="28"/>
+      <c r="N32" s="28"/>
+    </row>
+    <row r="33" spans="1:14">
+      <c r="A33" s="28"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="28"/>
+      <c r="H33" s="28"/>
+      <c r="I33" s="28"/>
+      <c r="J33" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="K33" s="28"/>
+      <c r="M33" s="28"/>
+      <c r="N33" s="28"/>
+    </row>
+    <row r="34" spans="1:14">
+      <c r="A34" s="28"/>
+      <c r="B34" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K34" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="L34" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M34" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
+      <c r="A35" s="28"/>
+      <c r="B35" s="37" t="s">
+        <v>162</v>
+      </c>
+      <c r="C35" s="28"/>
+      <c r="D35" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="E35" s="28"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="H35" s="28"/>
+      <c r="I35" s="28">
+        <v>2019</v>
+      </c>
+      <c r="J35" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="K35" s="28">
+        <v>1</v>
+      </c>
+      <c r="L35" s="28">
+        <v>0.6</v>
+      </c>
+      <c r="M35" s="28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
+      <c r="A36" s="28"/>
+      <c r="B36" s="28"/>
+      <c r="C36" s="28"/>
+      <c r="D36" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="E36" s="28"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="H36" s="28"/>
+      <c r="I36" s="28">
+        <v>2020</v>
+      </c>
+      <c r="J36" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="K36" s="28">
+        <v>1</v>
+      </c>
+      <c r="L36" s="28">
+        <v>2</v>
+      </c>
+      <c r="M36" s="28"/>
+    </row>
+    <row r="37" spans="1:14">
+      <c r="A37" s="28"/>
+      <c r="B37" s="28"/>
+      <c r="C37" s="28"/>
+      <c r="D37" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="E37" s="28"/>
+      <c r="F37" s="28"/>
+      <c r="G37" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="H37" s="28"/>
+      <c r="I37" s="28">
+        <v>2025</v>
+      </c>
+      <c r="J37" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="K37" s="28">
+        <v>1</v>
+      </c>
+      <c r="L37" s="28">
+        <v>2</v>
+      </c>
+      <c r="M37" s="28"/>
+    </row>
+    <row r="38" spans="1:14">
+      <c r="A38" s="28"/>
+      <c r="B38" s="28"/>
+      <c r="C38" s="28"/>
+      <c r="D38" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="E38" s="28"/>
+      <c r="F38" s="28"/>
+      <c r="G38" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="H38" s="28"/>
+      <c r="I38" s="28">
+        <v>2030</v>
+      </c>
+      <c r="J38" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="K38" s="28">
+        <v>1</v>
+      </c>
+      <c r="L38" s="28">
+        <v>2</v>
+      </c>
+      <c r="M38" s="28"/>
+    </row>
+    <row r="39" spans="1:14">
+      <c r="D39" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="E39" s="28"/>
+      <c r="F39" s="28"/>
+      <c r="G39" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="H39" s="28"/>
+      <c r="I39" s="28">
+        <v>2050</v>
+      </c>
+      <c r="J39" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="K39" s="28">
+        <v>1</v>
+      </c>
+      <c r="L39" s="28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="11:12">
+      <c r="L56" s="7"/>
+    </row>
+    <row r="57" spans="11:12">
+      <c r="L57" s="28"/>
+    </row>
+    <row r="58" spans="11:12">
+      <c r="K58" s="3"/>
+      <c r="L58" s="28"/>
+    </row>
+    <row r="59" spans="11:12">
+      <c r="K59" s="28"/>
+      <c r="L59" s="28"/>
+    </row>
+    <row r="60" spans="11:12">
+      <c r="K60" s="28"/>
+      <c r="L60" s="28"/>
+    </row>
+    <row r="61" spans="11:12">
+      <c r="K61" s="28"/>
+      <c r="L61" s="28"/>
+    </row>
+    <row r="62" spans="11:12">
+      <c r="K62" s="28"/>
+      <c r="L62" s="28"/>
+    </row>
+    <row r="63" spans="11:12">
+      <c r="K63" s="28"/>
+      <c r="L63" s="28"/>
+    </row>
+    <row r="64" spans="11:12">
+      <c r="K64" s="28"/>
+      <c r="L64" s="28"/>
+    </row>
+    <row r="65" spans="11:12">
+      <c r="K65" s="28"/>
+      <c r="L65" s="28"/>
+    </row>
+    <row r="66" spans="11:12">
+      <c r="K66" s="28"/>
+      <c r="L66" s="28"/>
+    </row>
+    <row r="67" spans="11:12">
+      <c r="L67" s="7"/>
+    </row>
+    <row r="68" spans="11:12">
+      <c r="L68" s="28"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3139,15 +3501,25 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:W21"/>
+  <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+      <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
@@ -3676,7 +4048,7 @@
       <c r="P16" s="28"/>
       <c r="Q16" s="28"/>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:21">
       <c r="A17" s="28"/>
       <c r="B17" s="6" t="s">
         <v>10</v>
@@ -3697,7 +4069,7 @@
       <c r="P17" s="28"/>
       <c r="Q17" s="28"/>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:21">
       <c r="A18" s="28"/>
       <c r="B18" s="28"/>
       <c r="C18" s="28"/>
@@ -3718,7 +4090,7 @@
       <c r="P18" s="28"/>
       <c r="Q18" s="28"/>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:21">
       <c r="A19" s="28"/>
       <c r="B19" s="5" t="s">
         <v>0</v>
@@ -3763,14 +4135,14 @@
       <c r="P19" s="28"/>
       <c r="Q19" s="28"/>
     </row>
-    <row r="20" spans="1:17">
+    <row r="20" spans="1:21">
       <c r="A20" s="28"/>
-      <c r="B20" s="28" t="s">
-        <v>159</v>
+      <c r="B20" s="37" t="s">
+        <v>163</v>
       </c>
       <c r="C20" s="28"/>
       <c r="D20" s="20" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E20" s="28"/>
       <c r="F20" s="28"/>
@@ -3779,7 +4151,7 @@
       </c>
       <c r="H20" s="28"/>
       <c r="I20" s="28">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="J20" s="28" t="s">
         <v>14</v>
@@ -3788,24 +4160,24 @@
         <v>1</v>
       </c>
       <c r="L20" s="28">
-        <v>1.03</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="M20" s="28">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="N20" s="28" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="O20" s="28"/>
       <c r="P20" s="28"/>
       <c r="Q20" s="28"/>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:21">
       <c r="A21" s="28"/>
       <c r="B21" s="28"/>
       <c r="C21" s="28"/>
       <c r="D21" s="20" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E21" s="28"/>
       <c r="F21" s="28"/>
@@ -3814,7 +4186,7 @@
       </c>
       <c r="H21" s="28"/>
       <c r="I21" s="28">
-        <v>2050</v>
+        <v>2020</v>
       </c>
       <c r="J21" s="28" t="s">
         <v>14</v>
@@ -3823,7 +4195,7 @@
         <v>1</v>
       </c>
       <c r="L21" s="28">
-        <v>7.5</v>
+        <v>1.03</v>
       </c>
       <c r="M21" s="3"/>
       <c r="N21" s="28"/>
@@ -3831,8 +4203,318 @@
       <c r="P21" s="28"/>
       <c r="Q21" s="28"/>
     </row>
+    <row r="22" spans="1:21">
+      <c r="D22" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="G22" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="H22" s="28"/>
+      <c r="I22" s="28">
+        <v>2025</v>
+      </c>
+      <c r="J22" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="K22" s="28">
+        <v>1</v>
+      </c>
+      <c r="L22" s="28">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21">
+      <c r="D23" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="G23" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="H23" s="28"/>
+      <c r="I23" s="28">
+        <v>2030</v>
+      </c>
+      <c r="J23" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="K23" s="28">
+        <v>1</v>
+      </c>
+      <c r="L23">
+        <v>3.78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" s="28" customFormat="1">
+      <c r="D24" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="G24" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="I24" s="28">
+        <v>2050</v>
+      </c>
+      <c r="J24" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="K24" s="28">
+        <v>1</v>
+      </c>
+      <c r="L24">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21">
+      <c r="A26" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="28"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="28"/>
+      <c r="I26" s="28"/>
+      <c r="J26" s="28"/>
+      <c r="K26" s="28"/>
+      <c r="L26" s="28"/>
+      <c r="M26" s="28"/>
+      <c r="N26" s="28"/>
+      <c r="O26" s="28"/>
+    </row>
+    <row r="27" spans="1:21">
+      <c r="A27" s="28"/>
+      <c r="B27" s="1" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,"~UC_Sets: R_E:",_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,"")))</f>
+        <v>~UC_Sets: R_E: IE,National</v>
+      </c>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="28"/>
+      <c r="J27" s="28"/>
+      <c r="K27" s="28"/>
+      <c r="L27" s="28"/>
+      <c r="M27" s="28"/>
+      <c r="N27" s="28"/>
+      <c r="O27" s="28"/>
+    </row>
+    <row r="28" spans="1:21">
+      <c r="A28" s="28"/>
+      <c r="B28" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="28"/>
+      <c r="K28" s="28"/>
+      <c r="L28" s="28"/>
+      <c r="M28" s="28"/>
+      <c r="N28" s="28"/>
+      <c r="O28" s="28"/>
+    </row>
+    <row r="29" spans="1:21">
+      <c r="A29" s="28"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="28"/>
+      <c r="I29" s="28"/>
+      <c r="J29" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="K29" s="28"/>
+      <c r="L29" s="28"/>
+      <c r="M29" s="28"/>
+      <c r="N29" s="28"/>
+      <c r="O29" s="28"/>
+    </row>
+    <row r="30" spans="1:21">
+      <c r="A30" s="28"/>
+      <c r="B30" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M30" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N30" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="O30" s="28"/>
+    </row>
+    <row r="31" spans="1:21">
+      <c r="A31" s="28"/>
+      <c r="B31" s="37" t="s">
+        <v>164</v>
+      </c>
+      <c r="C31" s="28"/>
+      <c r="D31" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="H31" s="28"/>
+      <c r="I31" s="28">
+        <v>2020</v>
+      </c>
+      <c r="J31" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="K31" s="28">
+        <v>1</v>
+      </c>
+      <c r="L31" s="28">
+        <v>1</v>
+      </c>
+      <c r="M31" s="28">
+        <v>5</v>
+      </c>
+      <c r="N31" s="28" t="s">
+        <v>159</v>
+      </c>
+      <c r="O31" s="28"/>
+      <c r="S31" s="28"/>
+      <c r="U31" s="26"/>
+    </row>
+    <row r="32" spans="1:21">
+      <c r="A32" s="28"/>
+      <c r="B32" s="28"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="E32" s="28"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="H32" s="28"/>
+      <c r="I32" s="28">
+        <v>2025</v>
+      </c>
+      <c r="J32" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="K32" s="28">
+        <v>1</v>
+      </c>
+      <c r="L32" s="28">
+        <v>1.67</v>
+      </c>
+      <c r="M32" s="3"/>
+      <c r="N32" s="28"/>
+      <c r="O32" s="28"/>
+      <c r="S32" s="28"/>
+      <c r="U32" s="26"/>
+    </row>
+    <row r="33" spans="1:21">
+      <c r="A33" s="28"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="H33" s="28"/>
+      <c r="I33" s="28">
+        <v>2030</v>
+      </c>
+      <c r="J33" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="K33" s="28">
+        <v>1</v>
+      </c>
+      <c r="L33" s="28">
+        <v>1.67</v>
+      </c>
+      <c r="M33" s="28"/>
+      <c r="N33" s="28"/>
+      <c r="O33" s="28"/>
+      <c r="S33" s="28"/>
+      <c r="U33" s="26"/>
+    </row>
+    <row r="34" spans="1:21">
+      <c r="A34" s="28"/>
+      <c r="B34" s="28"/>
+      <c r="C34" s="28"/>
+      <c r="D34" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="G34" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="H34" s="28"/>
+      <c r="I34" s="28">
+        <v>2050</v>
+      </c>
+      <c r="J34" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="K34" s="28">
+        <v>1</v>
+      </c>
+      <c r="L34" s="28">
+        <v>3.34</v>
+      </c>
+      <c r="M34" s="28"/>
+      <c r="N34" s="28"/>
+      <c r="O34" s="28"/>
+      <c r="S34" s="28"/>
+      <c r="U34" s="26"/>
+    </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -4148,7 +4830,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -5010,7 +5692,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -5147,7 +5829,7 @@
       <c r="M7" s="3"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Remove obsolete data input
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_PWR_RNW_Potentials.xlsx
+++ b/SuppXLS/Scen_PWR_RNW_Potentials.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_TIM\main-40\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF69CAF-1F32-4EB3-98F5-DFF8E253F98E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1131F433-F5DB-4714-8C86-CF1A5241A803}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34410" yWindow="-9135" windowWidth="28110" windowHeight="15885" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="6" r:id="rId1"/>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="167">
   <si>
     <t>UC_N</t>
   </si>
@@ -174,19 +174,16 @@
     <t>P-RNW-WIN-ON05</t>
   </si>
   <si>
-    <t>P-RNW-WIN-OF02</t>
-  </si>
-  <si>
     <t>P-RNW-SOL*</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>P-RNW-HYD*</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>P-RNW-OCE-WAV01</t>
     <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>P-RNW-HYD*</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>P-RNW-OCE-WAV01</t>
-    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Country</t>
@@ -362,11 +359,11 @@
   </si>
   <si>
     <t>P-RNW-OCE-TID02</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>P-RNW-SOL-CSP04</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Development</t>
@@ -579,41 +576,43 @@
     <t>P-RNW-WIN-OF0*</t>
   </si>
   <si>
-    <t>WIND_OFFSHORE_Socialy_Acceptable_Potential</t>
-  </si>
-  <si>
     <t>UC_NCAP</t>
   </si>
   <si>
-    <t>PWR_WONCAP</t>
-  </si>
-  <si>
-    <t>PWR_WONNCAP</t>
-  </si>
-  <si>
-    <t>PWR_WOFCAP</t>
-  </si>
-  <si>
-    <t>PWR_WOFNCAP</t>
+    <t>PWR_WOnCAP</t>
+  </si>
+  <si>
+    <t>PWR_WonNCAP</t>
+  </si>
+  <si>
+    <t>PWR_WOfCAP</t>
+  </si>
+  <si>
+    <t>PWR_WOfNCAP</t>
+  </si>
+  <si>
+    <t>Wind Offshore Socialy Acceptable Potential - Total</t>
+  </si>
+  <si>
+    <t>Wind Onshore Potential - Total</t>
+  </si>
+  <si>
+    <t>Wind Onshore Potential - New Capacity per Period</t>
+  </si>
+  <si>
+    <t>Wind Offshore Socialy Acceptable Potential - New Capacity per Period</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="31">
+  <fonts count="30">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1052,7 +1051,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -1173,17 +1172,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="hair">
-        <color indexed="64"/>
-      </top>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -1234,147 +1222,147 @@
   </borders>
   <cellStyleXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1382,12 +1370,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1398,19 +1385,19 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="30" fillId="36" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="36" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="36" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="29" fillId="36" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="37" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="37" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1910,729 +1897,729 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A3:AD37"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="28" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="28" customWidth="1"/>
-    <col min="3" max="3" width="3.140625" style="28" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" style="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" style="28" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5" style="28" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.7109375" style="28" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.85546875" style="28" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.42578125" style="28" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="5.7109375" style="28" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.5703125" style="28" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6" style="28" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.7109375" style="28" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.5703125" style="28" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.140625" style="28" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.7109375" style="28" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6" style="28" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.85546875" style="28" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.5703125" style="28" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.85546875" style="28" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.7109375" style="28" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="5" style="28" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.5703125" style="28" customWidth="1"/>
-    <col min="25" max="25" width="6.7109375" style="28" bestFit="1" customWidth="1"/>
-    <col min="26" max="28" width="6" style="28" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.7109375" style="28" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.7109375" style="28" bestFit="1" customWidth="1"/>
-    <col min="31" max="16384" width="9" style="28"/>
+    <col min="1" max="1" width="12.140625" style="27" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="27" customWidth="1"/>
+    <col min="3" max="3" width="3.140625" style="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" style="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" style="27" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5" style="27" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" style="27" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.85546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.42578125" style="27" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="5.7109375" style="27" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5703125" style="27" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6" style="27" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.7109375" style="27" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.5703125" style="27" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.140625" style="27" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.7109375" style="27" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6" style="27" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.85546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.5703125" style="27" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.85546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.7109375" style="27" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5" style="27" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.5703125" style="27" customWidth="1"/>
+    <col min="25" max="25" width="6.7109375" style="27" bestFit="1" customWidth="1"/>
+    <col min="26" max="28" width="6" style="27" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="5.7109375" style="27" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.7109375" style="27" bestFit="1" customWidth="1"/>
+    <col min="31" max="16384" width="9" style="27"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:30">
-      <c r="C3" s="29" t="str" cm="1">
+      <c r="C3" s="28" t="str" cm="1">
         <f t="array" ref="C3">INDEX(C5:C7,$A$4)</f>
         <v>IE</v>
       </c>
-      <c r="D3" s="29" t="str" cm="1">
+      <c r="D3" s="28" t="str" cm="1">
         <f t="array" ref="D3">INDEX(D5:D7,$A$4)</f>
         <v>National</v>
       </c>
-      <c r="E3" s="29" t="str" cm="1">
+      <c r="E3" s="28" t="str" cm="1">
         <f t="array" ref="E3">INDEX(E5:E7,$A$4)</f>
         <v>IE-CW</v>
       </c>
-      <c r="F3" s="29" t="str" cm="1">
+      <c r="F3" s="28" t="str" cm="1">
         <f t="array" ref="F3">INDEX(F5:F7,$A$4)</f>
         <v>IE-D</v>
       </c>
-      <c r="G3" s="29" t="str" cm="1">
+      <c r="G3" s="28" t="str" cm="1">
         <f t="array" ref="G3">INDEX(G5:G7,$A$4)</f>
         <v>IE-KE</v>
       </c>
-      <c r="H3" s="29" t="str" cm="1">
+      <c r="H3" s="28" t="str" cm="1">
         <f t="array" ref="H3">INDEX(H5:H7,$A$4)</f>
         <v>IE-KK</v>
       </c>
-      <c r="I3" s="29" t="str" cm="1">
+      <c r="I3" s="28" t="str" cm="1">
         <f t="array" ref="I3">INDEX(I5:I7,$A$4)</f>
         <v>IE-LS</v>
       </c>
-      <c r="J3" s="29" t="str" cm="1">
+      <c r="J3" s="28" t="str" cm="1">
         <f t="array" ref="J3">INDEX(J5:J7,$A$4)</f>
         <v>IE-LD</v>
       </c>
-      <c r="K3" s="29" t="str" cm="1">
+      <c r="K3" s="28" t="str" cm="1">
         <f t="array" ref="K3">INDEX(K5:K7,$A$4)</f>
         <v>IE-LH</v>
       </c>
-      <c r="L3" s="29" t="str" cm="1">
+      <c r="L3" s="28" t="str" cm="1">
         <f t="array" ref="L3">INDEX(L5:L7,$A$4)</f>
         <v>IE-MH</v>
       </c>
-      <c r="M3" s="29" t="str" cm="1">
+      <c r="M3" s="28" t="str" cm="1">
         <f t="array" ref="M3">INDEX(M5:M7,$A$4)</f>
         <v>IE-OY</v>
       </c>
-      <c r="N3" s="29" t="str" cm="1">
+      <c r="N3" s="28" t="str" cm="1">
         <f t="array" ref="N3">INDEX(N5:N7,$A$4)</f>
         <v>IE-WH</v>
       </c>
-      <c r="O3" s="29" t="str" cm="1">
+      <c r="O3" s="28" t="str" cm="1">
         <f t="array" ref="O3">INDEX(O5:O7,$A$4)</f>
         <v>IE-WX</v>
       </c>
-      <c r="P3" s="29" t="str" cm="1">
+      <c r="P3" s="28" t="str" cm="1">
         <f t="array" ref="P3">INDEX(P5:P7,$A$4)</f>
         <v>IE-WW</v>
       </c>
-      <c r="Q3" s="29" t="str" cm="1">
+      <c r="Q3" s="28" t="str" cm="1">
         <f t="array" ref="Q3">INDEX(Q5:Q7,$A$4)</f>
         <v>IE-CE</v>
       </c>
-      <c r="R3" s="29" t="str" cm="1">
+      <c r="R3" s="28" t="str" cm="1">
         <f t="array" ref="R3">INDEX(R5:R7,$A$4)</f>
         <v>IE-CO</v>
       </c>
-      <c r="S3" s="29" t="str" cm="1">
+      <c r="S3" s="28" t="str" cm="1">
         <f t="array" ref="S3">INDEX(S5:S7,$A$4)</f>
         <v>IE-KY</v>
       </c>
-      <c r="T3" s="29" t="str" cm="1">
+      <c r="T3" s="28" t="str" cm="1">
         <f t="array" ref="T3">INDEX(T5:T7,$A$4)</f>
         <v>IE-LK</v>
       </c>
-      <c r="U3" s="29" t="str" cm="1">
+      <c r="U3" s="28" t="str" cm="1">
         <f t="array" ref="U3">INDEX(U5:U7,$A$4)</f>
         <v>IE-TA</v>
       </c>
-      <c r="V3" s="29" t="str" cm="1">
+      <c r="V3" s="28" t="str" cm="1">
         <f t="array" ref="V3">INDEX(V5:V7,$A$4)</f>
         <v>IE-WD</v>
       </c>
-      <c r="W3" s="29" t="str" cm="1">
+      <c r="W3" s="28" t="str" cm="1">
         <f t="array" ref="W3">INDEX(W5:W7,$A$4)</f>
         <v>IE-G</v>
       </c>
-      <c r="X3" s="29" t="str" cm="1">
+      <c r="X3" s="28" t="str" cm="1">
         <f t="array" ref="X3">INDEX(X5:X7,$A$4)</f>
         <v>IE-LM</v>
       </c>
-      <c r="Y3" s="29" t="str" cm="1">
+      <c r="Y3" s="28" t="str" cm="1">
         <f t="array" ref="Y3">INDEX(Y5:Y7,$A$4)</f>
         <v>IE-MO</v>
       </c>
-      <c r="Z3" s="29" t="str" cm="1">
+      <c r="Z3" s="28" t="str" cm="1">
         <f t="array" ref="Z3">INDEX(Z5:Z7,$A$4)</f>
         <v>IE-RN</v>
       </c>
-      <c r="AA3" s="29" t="str" cm="1">
+      <c r="AA3" s="28" t="str" cm="1">
         <f t="array" ref="AA3">INDEX(AA5:AA7,$A$4)</f>
         <v>IE-SO</v>
       </c>
-      <c r="AB3" s="29" t="str" cm="1">
+      <c r="AB3" s="28" t="str" cm="1">
         <f t="array" ref="AB3">INDEX(AB5:AB7,$A$4)</f>
         <v>IE-CN</v>
       </c>
-      <c r="AC3" s="29" t="str" cm="1">
+      <c r="AC3" s="28" t="str" cm="1">
         <f t="array" ref="AC3">INDEX(AC5:AC7,$A$4)</f>
         <v>IE-DL</v>
       </c>
-      <c r="AD3" s="29" t="str" cm="1">
+      <c r="AD3" s="28" t="str" cm="1">
         <f t="array" ref="AD3">INDEX(AD5:AD7,$A$4)</f>
         <v>IE-MN</v>
       </c>
     </row>
     <row r="4" spans="1:30">
-      <c r="A4" s="28">
+      <c r="A4" s="27">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:30">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="C5" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="E5" s="29" t="str">
+      <c r="E5" s="28" t="str">
         <f>A11</f>
         <v>IE-CW</v>
       </c>
-      <c r="F5" s="29" t="str">
+      <c r="F5" s="28" t="str">
         <f>A16</f>
         <v>IE-D</v>
       </c>
-      <c r="G5" s="29" t="str">
+      <c r="G5" s="28" t="str">
         <f>A19</f>
         <v>IE-KE</v>
       </c>
-      <c r="H5" s="29" t="str">
+      <c r="H5" s="28" t="str">
         <f>A20</f>
         <v>IE-KK</v>
       </c>
-      <c r="I5" s="29" t="str">
+      <c r="I5" s="28" t="str">
         <f>A21</f>
         <v>IE-LS</v>
       </c>
-      <c r="J5" s="29" t="str">
+      <c r="J5" s="28" t="str">
         <f>A24</f>
         <v>IE-LD</v>
       </c>
-      <c r="K5" s="29" t="str">
+      <c r="K5" s="28" t="str">
         <f>A25</f>
         <v>IE-LH</v>
       </c>
-      <c r="L5" s="29" t="str">
+      <c r="L5" s="28" t="str">
         <f>A27</f>
         <v>IE-MH</v>
       </c>
-      <c r="M5" s="29" t="str">
+      <c r="M5" s="28" t="str">
         <f>A29</f>
         <v>IE-OY</v>
       </c>
-      <c r="N5" s="29" t="str">
+      <c r="N5" s="28" t="str">
         <f>A34</f>
         <v>IE-WH</v>
       </c>
-      <c r="O5" s="29" t="str">
+      <c r="O5" s="28" t="str">
         <f>A35</f>
         <v>IE-WX</v>
       </c>
-      <c r="P5" s="29" t="str">
+      <c r="P5" s="28" t="str">
         <f>A36</f>
         <v>IE-WW</v>
       </c>
-      <c r="Q5" s="29" t="str">
+      <c r="Q5" s="28" t="str">
         <f>A13</f>
         <v>IE-CE</v>
       </c>
-      <c r="R5" s="29" t="str">
+      <c r="R5" s="28" t="str">
         <f>A14</f>
         <v>IE-CO</v>
       </c>
-      <c r="S5" s="29" t="str">
+      <c r="S5" s="28" t="str">
         <f>A18</f>
         <v>IE-KY</v>
       </c>
-      <c r="T5" s="29" t="str">
+      <c r="T5" s="28" t="str">
         <f>A23</f>
         <v>IE-LK</v>
       </c>
-      <c r="U5" s="29" t="str">
+      <c r="U5" s="28" t="str">
         <f>A32</f>
         <v>IE-TA</v>
       </c>
-      <c r="V5" s="29" t="str">
+      <c r="V5" s="28" t="str">
         <f>A33</f>
         <v>IE-WD</v>
       </c>
-      <c r="W5" s="29" t="str">
+      <c r="W5" s="28" t="str">
         <f>A17</f>
         <v>IE-G</v>
       </c>
-      <c r="X5" s="29" t="str">
+      <c r="X5" s="28" t="str">
         <f>A22</f>
         <v>IE-LM</v>
       </c>
-      <c r="Y5" s="29" t="str">
+      <c r="Y5" s="28" t="str">
         <f>A26</f>
         <v>IE-MO</v>
       </c>
-      <c r="Z5" s="29" t="str">
+      <c r="Z5" s="28" t="str">
         <f>A30</f>
         <v>IE-RN</v>
       </c>
-      <c r="AA5" s="29" t="str">
+      <c r="AA5" s="28" t="str">
         <f>A31</f>
         <v>IE-SO</v>
       </c>
-      <c r="AB5" s="29" t="str">
+      <c r="AB5" s="28" t="str">
         <f>A12</f>
         <v>IE-CN</v>
       </c>
-      <c r="AC5" s="29" t="str">
+      <c r="AC5" s="28" t="str">
         <f>A15</f>
         <v>IE-DL</v>
       </c>
-      <c r="AD5" s="29" t="str">
+      <c r="AD5" s="28" t="str">
         <f>A28</f>
         <v>IE-MN</v>
       </c>
     </row>
     <row r="6" spans="1:30">
-      <c r="A6" s="28" t="s">
-        <v>97</v>
-      </c>
-      <c r="C6" s="29" t="str">
+      <c r="A6" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" s="28" t="str">
         <f>C5</f>
         <v>IE</v>
       </c>
-      <c r="D6" s="29" t="str">
+      <c r="D6" s="28" t="str">
         <f>"*"&amp;D5</f>
         <v>*National</v>
       </c>
-      <c r="E6" s="29" t="str">
+      <c r="E6" s="28" t="str">
         <f>"*"&amp;E5</f>
         <v>*IE-CW</v>
       </c>
-      <c r="F6" s="29" t="str">
+      <c r="F6" s="28" t="str">
         <f t="shared" ref="F6:AD6" si="0">"*"&amp;F5</f>
         <v>*IE-D</v>
       </c>
-      <c r="G6" s="29" t="str">
+      <c r="G6" s="28" t="str">
         <f t="shared" si="0"/>
         <v>*IE-KE</v>
       </c>
-      <c r="H6" s="29" t="str">
+      <c r="H6" s="28" t="str">
         <f t="shared" si="0"/>
         <v>*IE-KK</v>
       </c>
-      <c r="I6" s="29" t="str">
+      <c r="I6" s="28" t="str">
         <f t="shared" si="0"/>
         <v>*IE-LS</v>
       </c>
-      <c r="J6" s="29" t="str">
+      <c r="J6" s="28" t="str">
         <f t="shared" si="0"/>
         <v>*IE-LD</v>
       </c>
-      <c r="K6" s="29" t="str">
+      <c r="K6" s="28" t="str">
         <f t="shared" si="0"/>
         <v>*IE-LH</v>
       </c>
-      <c r="L6" s="29" t="str">
+      <c r="L6" s="28" t="str">
         <f t="shared" si="0"/>
         <v>*IE-MH</v>
       </c>
-      <c r="M6" s="29" t="str">
+      <c r="M6" s="28" t="str">
         <f t="shared" si="0"/>
         <v>*IE-OY</v>
       </c>
-      <c r="N6" s="29" t="str">
+      <c r="N6" s="28" t="str">
         <f t="shared" si="0"/>
         <v>*IE-WH</v>
       </c>
-      <c r="O6" s="29" t="str">
+      <c r="O6" s="28" t="str">
         <f t="shared" si="0"/>
         <v>*IE-WX</v>
       </c>
-      <c r="P6" s="29" t="str">
+      <c r="P6" s="28" t="str">
         <f t="shared" si="0"/>
         <v>*IE-WW</v>
       </c>
-      <c r="Q6" s="29" t="str">
+      <c r="Q6" s="28" t="str">
         <f t="shared" si="0"/>
         <v>*IE-CE</v>
       </c>
-      <c r="R6" s="29" t="str">
+      <c r="R6" s="28" t="str">
         <f t="shared" si="0"/>
         <v>*IE-CO</v>
       </c>
-      <c r="S6" s="29" t="str">
+      <c r="S6" s="28" t="str">
         <f t="shared" si="0"/>
         <v>*IE-KY</v>
       </c>
-      <c r="T6" s="29" t="str">
+      <c r="T6" s="28" t="str">
         <f t="shared" si="0"/>
         <v>*IE-LK</v>
       </c>
-      <c r="U6" s="29" t="str">
+      <c r="U6" s="28" t="str">
         <f t="shared" si="0"/>
         <v>*IE-TA</v>
       </c>
-      <c r="V6" s="29" t="str">
+      <c r="V6" s="28" t="str">
         <f t="shared" si="0"/>
         <v>*IE-WD</v>
       </c>
-      <c r="W6" s="29" t="str">
+      <c r="W6" s="28" t="str">
         <f t="shared" si="0"/>
         <v>*IE-G</v>
       </c>
-      <c r="X6" s="29" t="str">
+      <c r="X6" s="28" t="str">
         <f t="shared" si="0"/>
         <v>*IE-LM</v>
       </c>
-      <c r="Y6" s="29" t="str">
+      <c r="Y6" s="28" t="str">
         <f t="shared" si="0"/>
         <v>*IE-MO</v>
       </c>
-      <c r="Z6" s="29" t="str">
+      <c r="Z6" s="28" t="str">
         <f t="shared" si="0"/>
         <v>*IE-RN</v>
       </c>
-      <c r="AA6" s="29" t="str">
+      <c r="AA6" s="28" t="str">
         <f t="shared" si="0"/>
         <v>*IE-SO</v>
       </c>
-      <c r="AB6" s="29" t="str">
+      <c r="AB6" s="28" t="str">
         <f t="shared" si="0"/>
         <v>*IE-CN</v>
       </c>
-      <c r="AC6" s="29" t="str">
+      <c r="AC6" s="28" t="str">
         <f t="shared" si="0"/>
         <v>*IE-DL</v>
       </c>
-      <c r="AD6" s="29" t="str">
+      <c r="AD6" s="28" t="str">
         <f t="shared" si="0"/>
         <v>*IE-MN</v>
       </c>
     </row>
     <row r="7" spans="1:30">
-      <c r="A7" s="28" t="s">
-        <v>98</v>
-      </c>
-      <c r="C7" s="29" t="str">
+      <c r="A7" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" s="28" t="str">
         <f>"*"&amp;C5</f>
         <v>*IE</v>
       </c>
-      <c r="D7" s="29" t="str">
+      <c r="D7" s="28" t="str">
         <f>D5</f>
         <v>National</v>
       </c>
-      <c r="E7" s="29" t="str">
+      <c r="E7" s="28" t="str">
         <f t="shared" ref="E7:AD7" si="1">E5</f>
         <v>IE-CW</v>
       </c>
-      <c r="F7" s="29" t="str">
+      <c r="F7" s="28" t="str">
         <f t="shared" si="1"/>
         <v>IE-D</v>
       </c>
-      <c r="G7" s="29" t="str">
+      <c r="G7" s="28" t="str">
         <f t="shared" si="1"/>
         <v>IE-KE</v>
       </c>
-      <c r="H7" s="29" t="str">
+      <c r="H7" s="28" t="str">
         <f t="shared" si="1"/>
         <v>IE-KK</v>
       </c>
-      <c r="I7" s="29" t="str">
+      <c r="I7" s="28" t="str">
         <f t="shared" si="1"/>
         <v>IE-LS</v>
       </c>
-      <c r="J7" s="29" t="str">
+      <c r="J7" s="28" t="str">
         <f t="shared" si="1"/>
         <v>IE-LD</v>
       </c>
-      <c r="K7" s="29" t="str">
+      <c r="K7" s="28" t="str">
         <f t="shared" si="1"/>
         <v>IE-LH</v>
       </c>
-      <c r="L7" s="29" t="str">
+      <c r="L7" s="28" t="str">
         <f t="shared" si="1"/>
         <v>IE-MH</v>
       </c>
-      <c r="M7" s="29" t="str">
+      <c r="M7" s="28" t="str">
         <f t="shared" si="1"/>
         <v>IE-OY</v>
       </c>
-      <c r="N7" s="29" t="str">
+      <c r="N7" s="28" t="str">
         <f t="shared" si="1"/>
         <v>IE-WH</v>
       </c>
-      <c r="O7" s="29" t="str">
+      <c r="O7" s="28" t="str">
         <f t="shared" si="1"/>
         <v>IE-WX</v>
       </c>
-      <c r="P7" s="29" t="str">
+      <c r="P7" s="28" t="str">
         <f t="shared" si="1"/>
         <v>IE-WW</v>
       </c>
-      <c r="Q7" s="29" t="str">
+      <c r="Q7" s="28" t="str">
         <f t="shared" si="1"/>
         <v>IE-CE</v>
       </c>
-      <c r="R7" s="29" t="str">
+      <c r="R7" s="28" t="str">
         <f t="shared" si="1"/>
         <v>IE-CO</v>
       </c>
-      <c r="S7" s="29" t="str">
+      <c r="S7" s="28" t="str">
         <f t="shared" si="1"/>
         <v>IE-KY</v>
       </c>
-      <c r="T7" s="29" t="str">
+      <c r="T7" s="28" t="str">
         <f t="shared" si="1"/>
         <v>IE-LK</v>
       </c>
-      <c r="U7" s="29" t="str">
+      <c r="U7" s="28" t="str">
         <f t="shared" si="1"/>
         <v>IE-TA</v>
       </c>
-      <c r="V7" s="29" t="str">
+      <c r="V7" s="28" t="str">
         <f t="shared" si="1"/>
         <v>IE-WD</v>
       </c>
-      <c r="W7" s="29" t="str">
+      <c r="W7" s="28" t="str">
         <f t="shared" si="1"/>
         <v>IE-G</v>
       </c>
-      <c r="X7" s="29" t="str">
+      <c r="X7" s="28" t="str">
         <f t="shared" si="1"/>
         <v>IE-LM</v>
       </c>
-      <c r="Y7" s="29" t="str">
+      <c r="Y7" s="28" t="str">
         <f t="shared" si="1"/>
         <v>IE-MO</v>
       </c>
-      <c r="Z7" s="29" t="str">
+      <c r="Z7" s="28" t="str">
         <f t="shared" si="1"/>
         <v>IE-RN</v>
       </c>
-      <c r="AA7" s="29" t="str">
+      <c r="AA7" s="28" t="str">
         <f t="shared" si="1"/>
         <v>IE-SO</v>
       </c>
-      <c r="AB7" s="29" t="str">
+      <c r="AB7" s="28" t="str">
         <f t="shared" si="1"/>
         <v>IE-CN</v>
       </c>
-      <c r="AC7" s="29" t="str">
+      <c r="AC7" s="28" t="str">
         <f t="shared" si="1"/>
         <v>IE-DL</v>
       </c>
-      <c r="AD7" s="29" t="str">
+      <c r="AD7" s="28" t="str">
         <f t="shared" si="1"/>
         <v>IE-MN</v>
       </c>
     </row>
     <row r="10" spans="1:30" ht="15.75" thickBot="1">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="B10" s="31" t="s">
+    </row>
+    <row r="11" spans="1:30">
+      <c r="A11" s="31" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="11" spans="1:30">
-      <c r="A11" s="32" t="s">
+      <c r="B11" s="31" t="s">
         <v>101</v>
       </c>
-      <c r="B11" s="32" t="s">
+    </row>
+    <row r="12" spans="1:30">
+      <c r="A12" s="32" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="12" spans="1:30">
-      <c r="A12" s="33" t="s">
+      <c r="B12" s="32" t="s">
         <v>103</v>
       </c>
-      <c r="B12" s="33" t="s">
+    </row>
+    <row r="13" spans="1:30">
+      <c r="A13" s="32" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="13" spans="1:30">
-      <c r="A13" s="33" t="s">
+      <c r="B13" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="B13" s="33" t="s">
+    </row>
+    <row r="14" spans="1:30">
+      <c r="A14" s="32" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="14" spans="1:30">
-      <c r="A14" s="33" t="s">
+      <c r="B14" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="B14" s="33" t="s">
+    </row>
+    <row r="15" spans="1:30">
+      <c r="A15" s="32" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="15" spans="1:30">
-      <c r="A15" s="33" t="s">
+      <c r="B15" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="B15" s="33" t="s">
+    </row>
+    <row r="16" spans="1:30">
+      <c r="A16" s="32" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="16" spans="1:30">
-      <c r="A16" s="33" t="s">
+      <c r="B16" s="32" t="s">
         <v>111</v>
       </c>
-      <c r="B16" s="33" t="s">
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="32" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="33" t="s">
+      <c r="B17" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="B17" s="33" t="s">
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="32" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="33" t="s">
+      <c r="B18" s="32" t="s">
         <v>115</v>
       </c>
-      <c r="B18" s="33" t="s">
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="32" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="33" t="s">
+      <c r="B19" s="32" t="s">
         <v>117</v>
       </c>
-      <c r="B19" s="33" t="s">
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="32" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="33" t="s">
+      <c r="B20" s="32" t="s">
         <v>119</v>
       </c>
-      <c r="B20" s="33" t="s">
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="32" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="33" t="s">
+      <c r="B21" s="32" t="s">
         <v>121</v>
       </c>
-      <c r="B21" s="33" t="s">
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="32" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="33" t="s">
+      <c r="B22" s="32" t="s">
         <v>123</v>
       </c>
-      <c r="B22" s="33" t="s">
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="32" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="33" t="s">
+      <c r="B23" s="32" t="s">
         <v>125</v>
       </c>
-      <c r="B23" s="33" t="s">
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="32" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="33" t="s">
+      <c r="B24" s="32" t="s">
         <v>127</v>
       </c>
-      <c r="B24" s="33" t="s">
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="32" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="33" t="s">
+      <c r="B25" s="32" t="s">
         <v>129</v>
       </c>
-      <c r="B25" s="33" t="s">
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="32" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="33" t="s">
+      <c r="B26" s="32" t="s">
         <v>131</v>
       </c>
-      <c r="B26" s="33" t="s">
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="32" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="33" t="s">
+      <c r="B27" s="32" t="s">
         <v>133</v>
       </c>
-      <c r="B27" s="33" t="s">
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="32" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="33" t="s">
+      <c r="B28" s="32" t="s">
         <v>135</v>
       </c>
-      <c r="B28" s="33" t="s">
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="32" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="33" t="s">
+      <c r="B29" s="32" t="s">
         <v>137</v>
       </c>
-      <c r="B29" s="33" t="s">
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="32" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="33" t="s">
+      <c r="B30" s="32" t="s">
         <v>139</v>
       </c>
-      <c r="B30" s="33" t="s">
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="32" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="33" t="s">
+      <c r="B31" s="32" t="s">
         <v>141</v>
       </c>
-      <c r="B31" s="33" t="s">
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="32" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="33" t="s">
+      <c r="B32" s="32" t="s">
         <v>143</v>
       </c>
-      <c r="B32" s="33" t="s">
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="32" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="33" t="s">
+      <c r="B33" s="32" t="s">
         <v>145</v>
       </c>
-      <c r="B33" s="33" t="s">
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="32" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="33" t="s">
+      <c r="B34" s="32" t="s">
         <v>147</v>
       </c>
-      <c r="B34" s="33" t="s">
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="32" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="33" t="s">
+      <c r="B35" s="32" t="s">
         <v>149</v>
       </c>
-      <c r="B35" s="33" t="s">
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="32" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="33" t="s">
+      <c r="B36" s="32" t="s">
         <v>151</v>
       </c>
-      <c r="B36" s="33" t="s">
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="33" t="s">
         <v>152</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="34" t="s">
-        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -2674,23 +2661,27 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A2:N68"/>
+  <dimension ref="A2:M68"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="4" max="4" width="38.85546875" customWidth="1"/>
-    <col min="5" max="5" width="20.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:11">
       <c r="B2" s="10" t="s">
         <v>20</v>
       </c>
@@ -2704,7 +2695,7 @@
       <c r="J2" s="11"/>
       <c r="K2" s="12"/>
     </row>
-    <row r="3" spans="1:14" ht="15.75" thickBot="1">
+    <row r="3" spans="1:11" ht="15.75" thickBot="1">
       <c r="B3" s="13" t="s">
         <v>21</v>
       </c>
@@ -2738,7 +2729,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:11">
       <c r="C4" t="s">
         <v>14</v>
       </c>
@@ -2762,7 +2753,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:11">
       <c r="C5" t="s">
         <v>14</v>
       </c>
@@ -2783,7 +2774,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:11">
       <c r="C6" t="s">
         <v>14</v>
       </c>
@@ -2804,7 +2795,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:11">
       <c r="C7" t="s">
         <v>14</v>
       </c>
@@ -2825,44 +2816,44 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
-      <c r="B8" s="35"/>
-      <c r="C8" s="35" t="s">
+    <row r="8" spans="1:11">
+      <c r="B8" s="34"/>
+      <c r="C8" s="34" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="35">
+      <c r="E8" s="34">
         <v>2050</v>
       </c>
-      <c r="H8" s="35">
+      <c r="H8" s="34">
         <v>3.9907499999999998</v>
       </c>
-      <c r="I8" s="35">
+      <c r="I8" s="34">
         <f t="shared" si="0"/>
         <v>3.9907499999999998</v>
       </c>
-      <c r="K8" s="36" t="s">
+      <c r="K8" s="35" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
-      <c r="C9" s="28" t="s">
+    <row r="9" spans="1:11">
+      <c r="C9" s="27" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="28">
+      <c r="E9" s="27">
         <v>0</v>
       </c>
       <c r="F9" s="17"/>
       <c r="G9" s="17"/>
-      <c r="H9" s="28">
+      <c r="H9" s="27">
         <v>3</v>
       </c>
-      <c r="I9" s="28">
+      <c r="I9" s="27">
         <f>H9</f>
         <v>3</v>
       </c>
@@ -2871,177 +2862,165 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
-      <c r="C10" s="28" t="s">
+    <row r="10" spans="1:11">
+      <c r="C10" s="27" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="28">
+      <c r="E10" s="27">
         <v>0</v>
       </c>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28">
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27">
         <v>3</v>
       </c>
-      <c r="I10" s="28">
+      <c r="I10" s="27">
         <f t="shared" ref="I10:I13" si="1">H10</f>
         <v>3</v>
       </c>
-      <c r="J10" s="28"/>
+      <c r="J10" s="27"/>
       <c r="K10" s="20" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
-      <c r="C11" s="28" t="s">
+    <row r="11" spans="1:11">
+      <c r="C11" s="27" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="28">
+      <c r="E11" s="27">
         <v>0</v>
       </c>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28">
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27">
         <v>3</v>
       </c>
-      <c r="I11" s="28">
+      <c r="I11" s="27">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="J11" s="28"/>
+      <c r="J11" s="27"/>
       <c r="K11" s="20" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
-      <c r="C12" s="28" t="s">
+    <row r="12" spans="1:11">
+      <c r="C12" s="27" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="28">
+      <c r="E12" s="27">
         <v>0</v>
       </c>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28">
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27">
         <v>3</v>
       </c>
-      <c r="I12" s="28">
+      <c r="I12" s="27">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="J12" s="28"/>
+      <c r="J12" s="27"/>
       <c r="K12" s="20" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
-      <c r="C13" s="28" t="s">
+    <row r="13" spans="1:11">
+      <c r="C13" s="27" t="s">
         <v>14</v>
       </c>
       <c r="D13" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="28">
+      <c r="E13" s="27">
         <v>0</v>
       </c>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28">
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27">
         <v>3</v>
       </c>
-      <c r="I13" s="28">
+      <c r="I13" s="27">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="J13" s="28"/>
+      <c r="J13" s="27"/>
       <c r="K13" s="20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
-      <c r="A15" s="28" t="s">
+    <row r="15" spans="1:11">
+      <c r="A15" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="28"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="28"/>
-      <c r="M15" s="28"/>
-      <c r="N15" s="28"/>
-    </row>
-    <row r="16" spans="1:14">
-      <c r="A16" s="28"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="27"/>
       <c r="B16" s="1" t="str">
         <f>_xlfn.TEXTJOIN(" ",TRUE,"~UC_Sets: R_E:",_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,"")))</f>
         <v>~UC_Sets: R_E: IE,National</v>
       </c>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="28"/>
-      <c r="L16" s="28"/>
-      <c r="M16" s="28"/>
-      <c r="N16" s="28"/>
-    </row>
-    <row r="17" spans="1:14">
-      <c r="A17" s="28"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="27"/>
       <c r="B17" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="28"/>
-      <c r="L17" s="28"/>
-      <c r="M17" s="28"/>
-      <c r="N17" s="28"/>
-    </row>
-    <row r="18" spans="1:14">
-      <c r="A18" s="28"/>
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="28" t="s">
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="27"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="K18" s="28"/>
-      <c r="L18" s="28"/>
-      <c r="M18" s="28"/>
-      <c r="N18" s="28"/>
-    </row>
-    <row r="19" spans="1:14">
-      <c r="A19" s="28"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="27"/>
       <c r="B19" s="5" t="s">
         <v>0</v>
       </c>
@@ -3051,226 +3030,209 @@
       <c r="D19" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K19" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="27"/>
+      <c r="B20" s="36" t="s">
+        <v>159</v>
+      </c>
+      <c r="C20" s="27"/>
+      <c r="D20" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27">
+        <v>2019</v>
+      </c>
+      <c r="G20" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="27">
         <v>1</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G19" s="4" t="s">
+      <c r="I20" s="27">
+        <v>4</v>
+      </c>
+      <c r="J20" s="27">
         <v>5</v>
       </c>
-      <c r="H19" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="J19" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="K19" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="L19" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="M19" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14">
-      <c r="A20" s="28"/>
-      <c r="B20" s="37" t="s">
-        <v>161</v>
-      </c>
-      <c r="C20" s="28"/>
-      <c r="D20" s="20" t="s">
-        <v>156</v>
-      </c>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28" t="s">
+      <c r="K20" s="27" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="27"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28">
-        <v>2019</v>
-      </c>
-      <c r="J20" s="28" t="s">
+      <c r="E21" s="27"/>
+      <c r="F21" s="27">
+        <v>2020</v>
+      </c>
+      <c r="G21" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="K20" s="28">
+      <c r="H21" s="27">
         <v>1</v>
       </c>
-      <c r="L20" s="28">
-        <v>4</v>
-      </c>
-      <c r="M20" s="28">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14">
-      <c r="A21" s="28"/>
-      <c r="B21" s="28"/>
-      <c r="C21" s="28"/>
-      <c r="D21" s="20" t="s">
-        <v>156</v>
-      </c>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28" t="s">
+      <c r="I21" s="27">
+        <v>5.2</v>
+      </c>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="D22" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="H21" s="28"/>
-      <c r="I21" s="28">
-        <v>2020</v>
-      </c>
-      <c r="J21" s="28" t="s">
+      <c r="E22" s="27"/>
+      <c r="F22" s="27">
+        <v>2025</v>
+      </c>
+      <c r="G22" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="K21" s="28">
+      <c r="H22" s="27">
         <v>1</v>
       </c>
-      <c r="L21" s="28">
-        <v>5.2</v>
-      </c>
-      <c r="M21" s="28"/>
-    </row>
-    <row r="22" spans="1:14">
-      <c r="D22" s="20" t="s">
-        <v>156</v>
-      </c>
-      <c r="G22" s="28" t="s">
+      <c r="I22" s="27">
+        <v>5.5</v>
+      </c>
+      <c r="K22" s="27"/>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="D23" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="H22" s="28"/>
-      <c r="I22" s="28">
-        <v>2025</v>
-      </c>
-      <c r="J22" s="28" t="s">
+      <c r="E23" s="27"/>
+      <c r="F23" s="27">
+        <v>2030</v>
+      </c>
+      <c r="G23" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="K22" s="28">
+      <c r="H23" s="27">
         <v>1</v>
       </c>
-      <c r="L22" s="28">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14">
-      <c r="D23" s="20" t="s">
-        <v>156</v>
-      </c>
-      <c r="G23" s="28" t="s">
+      <c r="I23" s="27">
+        <v>5.9</v>
+      </c>
+      <c r="K23" s="27"/>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="D24" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="H23" s="28"/>
-      <c r="I23" s="28">
-        <v>2030</v>
-      </c>
-      <c r="J23" s="28" t="s">
+      <c r="E24" s="27"/>
+      <c r="F24" s="27">
+        <v>2050</v>
+      </c>
+      <c r="G24" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="K23" s="28">
+      <c r="H24" s="27">
         <v>1</v>
       </c>
-      <c r="L23" s="28">
-        <v>5.9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14">
-      <c r="D24" s="20" t="s">
-        <v>156</v>
-      </c>
-      <c r="G24" s="28" t="s">
-        <v>155</v>
-      </c>
-      <c r="H24" s="28"/>
-      <c r="I24" s="28">
-        <v>2050</v>
-      </c>
-      <c r="J24" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="K24" s="28">
-        <v>1</v>
-      </c>
-      <c r="L24" s="28">
+      <c r="I24" s="27">
         <v>6.9</v>
       </c>
-    </row>
-    <row r="30" spans="1:14">
-      <c r="A30" s="28" t="s">
+      <c r="K24" s="27"/>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="K25" s="27"/>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="K26" s="27"/>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="K27" s="27"/>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="K28" s="27"/>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="K29" s="27"/>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="28"/>
-      <c r="H30" s="28"/>
-      <c r="I30" s="28"/>
-      <c r="J30" s="28"/>
-      <c r="K30" s="28"/>
-      <c r="M30" s="28"/>
-      <c r="N30" s="28"/>
-    </row>
-    <row r="31" spans="1:14">
-      <c r="A31" s="28"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="J30" s="27"/>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" s="27"/>
       <c r="B31" s="1" t="str">
         <f>_xlfn.TEXTJOIN(" ",TRUE,"~UC_Sets: R_E:",_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,"")))</f>
         <v>~UC_Sets: R_E: IE,National</v>
       </c>
-      <c r="C31" s="28"/>
-      <c r="D31" s="28"/>
-      <c r="E31" s="28"/>
-      <c r="F31" s="28"/>
-      <c r="G31" s="28"/>
-      <c r="H31" s="28"/>
-      <c r="I31" s="28"/>
-      <c r="J31" s="28"/>
-      <c r="K31" s="28"/>
-      <c r="M31" s="28"/>
-      <c r="N31" s="28"/>
-    </row>
-    <row r="32" spans="1:14">
-      <c r="A32" s="28"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
+      <c r="J31" s="27"/>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32" s="27"/>
       <c r="B32" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C32" s="28"/>
-      <c r="D32" s="28"/>
-      <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="28"/>
-      <c r="H32" s="28"/>
-      <c r="I32" s="28"/>
-      <c r="J32" s="28"/>
-      <c r="K32" s="28"/>
-      <c r="M32" s="28"/>
-      <c r="N32" s="28"/>
-    </row>
-    <row r="33" spans="1:14">
-      <c r="A33" s="28"/>
-      <c r="B33" s="28"/>
-      <c r="C33" s="28"/>
-      <c r="D33" s="28"/>
-      <c r="E33" s="28"/>
-      <c r="F33" s="28"/>
-      <c r="G33" s="28"/>
-      <c r="H33" s="28"/>
-      <c r="I33" s="28"/>
-      <c r="J33" s="28" t="s">
+      <c r="C32" s="27"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="27"/>
+      <c r="G32" s="27"/>
+      <c r="H32" s="27"/>
+      <c r="J32" s="27"/>
+      <c r="K32" s="27"/>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="A33" s="27"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="27"/>
+      <c r="G33" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="K33" s="28"/>
-      <c r="M33" s="28"/>
-      <c r="N33" s="28"/>
-    </row>
-    <row r="34" spans="1:14">
-      <c r="A34" s="28"/>
+      <c r="H33" s="27"/>
+      <c r="J33" s="27"/>
+      <c r="K33" s="27"/>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34" s="27"/>
       <c r="B34" s="5" t="s">
         <v>0</v>
       </c>
@@ -3280,219 +3242,170 @@
       <c r="D34" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="E34" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J34" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K34" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" s="27"/>
+      <c r="B35" s="36" t="s">
+        <v>160</v>
+      </c>
+      <c r="C35" s="27"/>
+      <c r="D35" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="E35" s="27"/>
+      <c r="F35" s="27">
+        <v>2019</v>
+      </c>
+      <c r="G35" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="H35" s="27">
         <v>1</v>
       </c>
-      <c r="F34" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G34" s="4" t="s">
+      <c r="I35" s="27">
+        <v>0.6</v>
+      </c>
+      <c r="J35" s="27">
         <v>5</v>
       </c>
-      <c r="H34" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I34" s="4" t="s">
+      <c r="K35" s="27" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" s="27"/>
+      <c r="B36" s="27"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="E36" s="27"/>
+      <c r="F36" s="27">
+        <v>2020</v>
+      </c>
+      <c r="G36" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="H36" s="27">
+        <v>1</v>
+      </c>
+      <c r="I36" s="27">
         <v>2</v>
       </c>
-      <c r="J34" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="K34" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="L34" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="M34" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14">
-      <c r="A35" s="28"/>
-      <c r="B35" s="37" t="s">
-        <v>162</v>
-      </c>
-      <c r="C35" s="28"/>
-      <c r="D35" s="20" t="s">
-        <v>156</v>
-      </c>
-      <c r="E35" s="28"/>
-      <c r="F35" s="28"/>
-      <c r="G35" s="28" t="s">
-        <v>155</v>
-      </c>
-      <c r="H35" s="28"/>
-      <c r="I35" s="28">
-        <v>2019</v>
-      </c>
-      <c r="J35" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="K35" s="28">
-        <v>1</v>
-      </c>
-      <c r="L35" s="28">
-        <v>0.6</v>
-      </c>
-      <c r="M35" s="28">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14">
-      <c r="A36" s="28"/>
-      <c r="B36" s="28"/>
-      <c r="C36" s="28"/>
-      <c r="D36" s="20" t="s">
-        <v>156</v>
-      </c>
-      <c r="E36" s="28"/>
-      <c r="F36" s="28"/>
-      <c r="G36" s="28" t="s">
-        <v>155</v>
-      </c>
-      <c r="H36" s="28"/>
-      <c r="I36" s="28">
-        <v>2020</v>
-      </c>
-      <c r="J36" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="K36" s="28">
-        <v>1</v>
-      </c>
-      <c r="L36" s="28">
-        <v>2</v>
-      </c>
-      <c r="M36" s="28"/>
-    </row>
-    <row r="37" spans="1:14">
-      <c r="A37" s="28"/>
-      <c r="B37" s="28"/>
-      <c r="C37" s="28"/>
-      <c r="D37" s="20" t="s">
-        <v>156</v>
-      </c>
-      <c r="E37" s="28"/>
-      <c r="F37" s="28"/>
-      <c r="G37" s="28" t="s">
-        <v>155</v>
-      </c>
-      <c r="H37" s="28"/>
-      <c r="I37" s="28">
-        <v>2025</v>
-      </c>
-      <c r="J37" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="K37" s="28">
-        <v>1</v>
-      </c>
-      <c r="L37" s="28">
-        <v>2</v>
-      </c>
-      <c r="M37" s="28"/>
-    </row>
-    <row r="38" spans="1:14">
-      <c r="A38" s="28"/>
-      <c r="B38" s="28"/>
-      <c r="C38" s="28"/>
-      <c r="D38" s="20" t="s">
-        <v>156</v>
-      </c>
-      <c r="E38" s="28"/>
-      <c r="F38" s="28"/>
-      <c r="G38" s="28" t="s">
-        <v>155</v>
-      </c>
-      <c r="H38" s="28"/>
-      <c r="I38" s="28">
-        <v>2030</v>
-      </c>
-      <c r="J38" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="K38" s="28">
-        <v>1</v>
-      </c>
-      <c r="L38" s="28">
-        <v>2</v>
-      </c>
-      <c r="M38" s="28"/>
-    </row>
-    <row r="39" spans="1:14">
-      <c r="D39" s="20" t="s">
-        <v>156</v>
-      </c>
-      <c r="E39" s="28"/>
-      <c r="F39" s="28"/>
-      <c r="G39" s="28" t="s">
-        <v>155</v>
-      </c>
-      <c r="H39" s="28"/>
-      <c r="I39" s="28">
-        <v>2050</v>
-      </c>
-      <c r="J39" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="K39" s="28">
-        <v>1</v>
-      </c>
-      <c r="L39" s="28">
-        <v>2</v>
-      </c>
+      <c r="J36" s="27"/>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" s="27"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
+      <c r="G37" s="27"/>
+      <c r="H37" s="27"/>
+      <c r="I37" s="27"/>
+      <c r="J37" s="27"/>
+      <c r="K37" s="27"/>
+      <c r="L37" s="27"/>
+      <c r="M37" s="27"/>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38" s="27"/>
+      <c r="B38" s="27"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="27"/>
+      <c r="F38" s="27"/>
+      <c r="G38" s="27"/>
+      <c r="H38" s="27"/>
+      <c r="I38" s="27"/>
+      <c r="J38" s="27"/>
+      <c r="K38" s="27"/>
+      <c r="L38" s="27"/>
+      <c r="M38" s="27"/>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="D39" s="20"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="27"/>
+      <c r="G39" s="27"/>
+      <c r="H39" s="27"/>
+      <c r="I39" s="27"/>
+      <c r="J39" s="27"/>
+      <c r="K39" s="27"/>
+      <c r="L39" s="27"/>
     </row>
     <row r="56" spans="11:12">
       <c r="L56" s="7"/>
     </row>
     <row r="57" spans="11:12">
-      <c r="L57" s="28"/>
+      <c r="L57" s="27"/>
     </row>
     <row r="58" spans="11:12">
       <c r="K58" s="3"/>
-      <c r="L58" s="28"/>
+      <c r="L58" s="27"/>
     </row>
     <row r="59" spans="11:12">
-      <c r="K59" s="28"/>
-      <c r="L59" s="28"/>
+      <c r="K59" s="27"/>
+      <c r="L59" s="27"/>
     </row>
     <row r="60" spans="11:12">
-      <c r="K60" s="28"/>
-      <c r="L60" s="28"/>
+      <c r="K60" s="27"/>
+      <c r="L60" s="27"/>
     </row>
     <row r="61" spans="11:12">
-      <c r="K61" s="28"/>
-      <c r="L61" s="28"/>
+      <c r="K61" s="27"/>
+      <c r="L61" s="27"/>
     </row>
     <row r="62" spans="11:12">
-      <c r="K62" s="28"/>
-      <c r="L62" s="28"/>
+      <c r="K62" s="27"/>
+      <c r="L62" s="27"/>
     </row>
     <row r="63" spans="11:12">
-      <c r="K63" s="28"/>
-      <c r="L63" s="28"/>
+      <c r="K63" s="27"/>
+      <c r="L63" s="27"/>
     </row>
     <row r="64" spans="11:12">
-      <c r="K64" s="28"/>
-      <c r="L64" s="28"/>
+      <c r="K64" s="27"/>
+      <c r="L64" s="27"/>
     </row>
     <row r="65" spans="11:12">
-      <c r="K65" s="28"/>
-      <c r="L65" s="28"/>
+      <c r="K65" s="27"/>
+      <c r="L65" s="27"/>
     </row>
     <row r="66" spans="11:12">
-      <c r="K66" s="28"/>
-      <c r="L66" s="28"/>
+      <c r="K66" s="27"/>
+      <c r="L66" s="27"/>
     </row>
     <row r="67" spans="11:12">
       <c r="L67" s="7"/>
     </row>
     <row r="68" spans="11:12">
-      <c r="L68" s="28"/>
+      <c r="L68" s="27"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3501,10 +3414,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:W34"/>
+  <dimension ref="A2:W34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L35" sqref="L35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3514,463 +3427,512 @@
     <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
-      <c r="B1" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="12"/>
-    </row>
-    <row r="2" spans="1:23" ht="15.75" thickBot="1">
-      <c r="B2" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="14" t="str">
-        <f>Regions!C3</f>
-        <v>IE</v>
-      </c>
-      <c r="I2" s="14" t="str">
-        <f>Regions!D3</f>
-        <v>National</v>
-      </c>
-      <c r="J2" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="K2" s="15" t="s">
-        <v>3</v>
-      </c>
+    <row r="2" spans="1:23">
+      <c r="A2" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
       <c r="N2" t="s">
+        <v>35</v>
+      </c>
+      <c r="O2" t="s">
         <v>36</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>37</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>39</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>40</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>41</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>42</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>43</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>44</v>
       </c>
-      <c r="W2" t="s">
+    </row>
+    <row r="3" spans="1:23">
+      <c r="A3" s="27"/>
+      <c r="B3" s="1" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,"~UC_Sets: R_E:",_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,"")))</f>
+        <v>~UC_Sets: R_E: IE,National</v>
+      </c>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+      <c r="N3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="3" spans="1:23">
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3">
-        <v>2020</v>
-      </c>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3">
-        <v>1.0298</v>
-      </c>
-      <c r="I3">
-        <f>H3</f>
-        <v>1.0298</v>
-      </c>
-      <c r="J3" s="17"/>
-      <c r="K3" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>46</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>47</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>48</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>49</v>
       </c>
       <c r="R3">
         <v>100</v>
       </c>
       <c r="S3" t="s">
+        <v>49</v>
+      </c>
+      <c r="T3" t="s">
         <v>50</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>51</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>52</v>
-      </c>
-      <c r="V3" t="s">
-        <v>53</v>
       </c>
       <c r="W3">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:23">
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4">
-        <v>2025</v>
-      </c>
-      <c r="H4">
-        <v>2.6998000000000002</v>
-      </c>
-      <c r="I4" s="16">
-        <f t="shared" ref="I4:I6" si="0">H4</f>
-        <v>2.6998000000000002</v>
-      </c>
-      <c r="K4" s="23" t="s">
-        <v>32</v>
-      </c>
+      <c r="A4" s="27"/>
+      <c r="B4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="27"/>
       <c r="N4" t="s">
+        <v>45</v>
+      </c>
+      <c r="O4" t="s">
         <v>46</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>47</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>48</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>49</v>
       </c>
       <c r="R4">
         <v>100</v>
       </c>
       <c r="S4" t="s">
+        <v>49</v>
+      </c>
+      <c r="T4" t="s">
         <v>50</v>
       </c>
-      <c r="T4" t="s">
-        <v>51</v>
-      </c>
       <c r="U4" t="s">
+        <v>53</v>
+      </c>
+      <c r="V4" t="s">
         <v>54</v>
-      </c>
-      <c r="V4" t="s">
-        <v>55</v>
       </c>
       <c r="W4">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:23">
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5">
-        <v>2030</v>
-      </c>
-      <c r="H5">
-        <v>3.4620000000000002</v>
-      </c>
-      <c r="I5" s="16">
-        <f t="shared" si="0"/>
-        <v>3.4620000000000002</v>
-      </c>
-      <c r="K5" s="23" t="s">
-        <v>32</v>
-      </c>
+      <c r="A5" s="27"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
+      <c r="L5" s="27"/>
       <c r="N5" t="s">
+        <v>45</v>
+      </c>
+      <c r="O5" t="s">
         <v>46</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>47</v>
       </c>
-      <c r="P5" t="s">
-        <v>48</v>
-      </c>
       <c r="Q5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="R5">
         <v>100</v>
       </c>
       <c r="S5" t="s">
+        <v>49</v>
+      </c>
+      <c r="T5" t="s">
         <v>50</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>51</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>52</v>
-      </c>
-      <c r="V5" t="s">
-        <v>53</v>
       </c>
       <c r="W5">
         <v>0.75</v>
       </c>
     </row>
     <row r="6" spans="1:23">
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6">
-        <v>2050</v>
-      </c>
-      <c r="H6">
-        <v>3.4620000000000002</v>
-      </c>
-      <c r="I6" s="16">
-        <f t="shared" si="0"/>
-        <v>3.4620000000000002</v>
-      </c>
-      <c r="K6" s="23" t="s">
-        <v>32</v>
-      </c>
+      <c r="A6" s="27"/>
+      <c r="B6" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L6" s="27"/>
       <c r="N6" t="s">
+        <v>45</v>
+      </c>
+      <c r="O6" t="s">
         <v>46</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>47</v>
       </c>
-      <c r="P6" t="s">
-        <v>48</v>
-      </c>
       <c r="Q6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="R6">
         <v>100</v>
       </c>
       <c r="S6" t="s">
+        <v>49</v>
+      </c>
+      <c r="T6" t="s">
         <v>50</v>
       </c>
-      <c r="T6" t="s">
-        <v>51</v>
-      </c>
       <c r="U6" t="s">
+        <v>53</v>
+      </c>
+      <c r="V6" t="s">
         <v>54</v>
-      </c>
-      <c r="V6" t="s">
-        <v>55</v>
       </c>
       <c r="W6">
         <v>3.4620000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:23">
-      <c r="C7" t="s">
+      <c r="A7" s="27"/>
+      <c r="B7" s="36" t="s">
+        <v>161</v>
+      </c>
+      <c r="C7" s="27"/>
+      <c r="D7" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27">
+        <v>2019</v>
+      </c>
+      <c r="G7" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="H7">
+      <c r="H7" s="27">
+        <v>1</v>
+      </c>
+      <c r="I7" s="27">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="J7" s="27">
         <v>5</v>
       </c>
-      <c r="I7">
-        <v>5</v>
-      </c>
-      <c r="K7" s="23" t="s">
-        <v>32</v>
-      </c>
+      <c r="K7" s="27" t="s">
+        <v>163</v>
+      </c>
+      <c r="L7" s="27"/>
       <c r="N7" t="s">
+        <v>45</v>
+      </c>
+      <c r="O7" t="s">
         <v>46</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>47</v>
       </c>
-      <c r="P7" t="s">
-        <v>48</v>
-      </c>
       <c r="Q7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="R7">
         <v>100</v>
       </c>
       <c r="S7" t="s">
+        <v>49</v>
+      </c>
+      <c r="T7" t="s">
         <v>50</v>
       </c>
-      <c r="T7" t="s">
+      <c r="U7" t="s">
         <v>51</v>
       </c>
-      <c r="U7" t="s">
+      <c r="V7" t="s">
         <v>52</v>
-      </c>
-      <c r="V7" t="s">
-        <v>53</v>
       </c>
       <c r="W7">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:23">
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27">
+        <v>2020</v>
+      </c>
+      <c r="G8" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="27">
+        <v>1</v>
+      </c>
+      <c r="I8" s="27">
+        <v>1.03</v>
+      </c>
+      <c r="J8" s="3"/>
+      <c r="K8" s="27"/>
+      <c r="L8" s="27"/>
       <c r="N8" t="s">
+        <v>45</v>
+      </c>
+      <c r="O8" t="s">
         <v>46</v>
       </c>
-      <c r="O8" t="s">
+      <c r="P8" t="s">
         <v>47</v>
       </c>
-      <c r="P8" t="s">
-        <v>48</v>
-      </c>
       <c r="Q8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="R8">
         <v>100</v>
       </c>
       <c r="S8" t="s">
+        <v>49</v>
+      </c>
+      <c r="T8" t="s">
         <v>50</v>
       </c>
-      <c r="T8" t="s">
-        <v>51</v>
-      </c>
       <c r="U8" t="s">
+        <v>53</v>
+      </c>
+      <c r="V8" t="s">
         <v>54</v>
-      </c>
-      <c r="V8" t="s">
-        <v>55</v>
       </c>
       <c r="W8">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:23">
+      <c r="D9" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27">
+        <v>2025</v>
+      </c>
+      <c r="G9" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="27">
+        <v>1</v>
+      </c>
+      <c r="I9" s="27">
+        <v>2.7</v>
+      </c>
       <c r="N9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O9" t="s">
+        <v>57</v>
+      </c>
+      <c r="P9" t="s">
         <v>58</v>
-      </c>
-      <c r="P9" t="s">
-        <v>59</v>
       </c>
       <c r="R9">
         <v>100</v>
       </c>
       <c r="S9" t="s">
+        <v>49</v>
+      </c>
+      <c r="T9" t="s">
         <v>50</v>
       </c>
-      <c r="T9" t="s">
+      <c r="U9" t="s">
         <v>51</v>
       </c>
-      <c r="U9" t="s">
+      <c r="V9" t="s">
         <v>52</v>
-      </c>
-      <c r="V9" t="s">
-        <v>53</v>
       </c>
       <c r="W9">
         <v>35.200000000000003</v>
       </c>
     </row>
     <row r="10" spans="1:23">
+      <c r="D10" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27">
+        <v>2030</v>
+      </c>
+      <c r="G10" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="27">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>3.78</v>
+      </c>
       <c r="N10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R10">
         <v>100</v>
       </c>
       <c r="S10" t="s">
+        <v>49</v>
+      </c>
+      <c r="T10" t="s">
         <v>50</v>
       </c>
-      <c r="T10" t="s">
+      <c r="U10" t="s">
         <v>51</v>
       </c>
-      <c r="U10" t="s">
+      <c r="V10" t="s">
         <v>52</v>
-      </c>
-      <c r="V10" t="s">
-        <v>53</v>
       </c>
       <c r="W10">
         <v>35.700000000000003</v>
       </c>
     </row>
     <row r="11" spans="1:23">
+      <c r="A11" s="27"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27">
+        <v>2050</v>
+      </c>
+      <c r="G11" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="27">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>7.5</v>
+      </c>
+      <c r="J11" s="27"/>
+      <c r="K11" s="27"/>
+      <c r="L11" s="27"/>
       <c r="N11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O11" t="s">
+        <v>57</v>
+      </c>
+      <c r="P11" t="s">
         <v>58</v>
-      </c>
-      <c r="P11" t="s">
-        <v>59</v>
       </c>
       <c r="R11">
         <v>100</v>
       </c>
       <c r="S11" t="s">
+        <v>49</v>
+      </c>
+      <c r="T11" t="s">
         <v>50</v>
       </c>
-      <c r="T11" t="s">
-        <v>51</v>
-      </c>
       <c r="U11" t="s">
+        <v>53</v>
+      </c>
+      <c r="V11" t="s">
         <v>54</v>
-      </c>
-      <c r="V11" t="s">
-        <v>55</v>
       </c>
       <c r="W11">
         <v>137.4</v>
@@ -3978,543 +3940,280 @@
     </row>
     <row r="12" spans="1:23">
       <c r="N12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R12">
         <v>100</v>
       </c>
       <c r="S12" t="s">
+        <v>49</v>
+      </c>
+      <c r="T12" t="s">
         <v>50</v>
       </c>
-      <c r="T12" t="s">
-        <v>51</v>
-      </c>
       <c r="U12" t="s">
+        <v>53</v>
+      </c>
+      <c r="V12" t="s">
         <v>54</v>
-      </c>
-      <c r="V12" t="s">
-        <v>55</v>
       </c>
       <c r="W12">
         <v>139.9</v>
       </c>
     </row>
-    <row r="15" spans="1:23">
-      <c r="A15" s="28" t="s">
+    <row r="13" spans="1:23">
+      <c r="A13" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="28"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="28"/>
-      <c r="M15" s="28"/>
-      <c r="N15" s="28"/>
-      <c r="O15" s="28"/>
-      <c r="P15" s="28"/>
-      <c r="Q15" s="28"/>
-    </row>
-    <row r="16" spans="1:23">
-      <c r="A16" s="28"/>
-      <c r="B16" s="1" t="str">
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="27"/>
+      <c r="L13" s="27"/>
+    </row>
+    <row r="14" spans="1:23">
+      <c r="A14" s="27"/>
+      <c r="B14" s="1" t="str">
         <f>_xlfn.TEXTJOIN(" ",TRUE,"~UC_Sets: R_E:",_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,"")))</f>
         <v>~UC_Sets: R_E: IE,National</v>
       </c>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="28"/>
-      <c r="L16" s="28"/>
-      <c r="M16" s="28"/>
-      <c r="N16" s="28"/>
-      <c r="O16" s="28"/>
-      <c r="P16" s="28"/>
-      <c r="Q16" s="28"/>
-    </row>
-    <row r="17" spans="1:21">
-      <c r="A17" s="28"/>
-      <c r="B17" s="6" t="s">
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="27"/>
+    </row>
+    <row r="15" spans="1:23">
+      <c r="A15" s="27"/>
+      <c r="B15" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="28"/>
-      <c r="L17" s="28"/>
-      <c r="M17" s="28"/>
-      <c r="N17" s="28"/>
-      <c r="O17" s="28"/>
-      <c r="P17" s="28"/>
-      <c r="Q17" s="28"/>
-    </row>
-    <row r="18" spans="1:21">
-      <c r="A18" s="28"/>
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="28" t="s">
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
+      <c r="L15" s="27"/>
+      <c r="M15" s="27"/>
+      <c r="N15" s="27"/>
+    </row>
+    <row r="16" spans="1:23">
+      <c r="A16" s="27"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="K18" s="28"/>
-      <c r="L18" s="28"/>
-      <c r="M18" s="28"/>
-      <c r="N18" s="28"/>
-      <c r="O18" s="28"/>
-      <c r="P18" s="28"/>
-      <c r="Q18" s="28"/>
-    </row>
-    <row r="19" spans="1:21">
-      <c r="A19" s="28"/>
-      <c r="B19" s="5" t="s">
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="27"/>
+      <c r="N16" s="27"/>
+    </row>
+    <row r="17" spans="1:18">
+      <c r="A17" s="27"/>
+      <c r="B17" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L17" s="27"/>
+      <c r="M17" s="27"/>
+      <c r="N17" s="27"/>
+    </row>
+    <row r="18" spans="1:18">
+      <c r="A18" s="27"/>
+      <c r="B18" s="36" t="s">
+        <v>162</v>
+      </c>
+      <c r="C18" s="27"/>
+      <c r="D18" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27">
+        <v>2020</v>
+      </c>
+      <c r="G18" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" s="27">
         <v>1</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G19" s="4" t="s">
+      <c r="I18" s="27">
+        <v>1</v>
+      </c>
+      <c r="J18" s="27">
         <v>5</v>
       </c>
-      <c r="H19" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="J19" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="K19" s="3" t="s">
+      <c r="K18" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="L18" s="27"/>
+      <c r="M18" s="27"/>
+      <c r="N18" s="27"/>
+    </row>
+    <row r="19" spans="1:18">
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="L19" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="M19" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="N19" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="O19" s="28"/>
-      <c r="P19" s="28"/>
-      <c r="Q19" s="28"/>
-    </row>
-    <row r="20" spans="1:21">
-      <c r="A20" s="28"/>
-      <c r="B20" s="37" t="s">
-        <v>163</v>
-      </c>
-      <c r="C20" s="28"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27">
+        <v>2025</v>
+      </c>
+      <c r="G19" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="27">
+        <v>1</v>
+      </c>
+      <c r="I19" s="27">
+        <v>1.67</v>
+      </c>
+      <c r="J19" s="3"/>
+      <c r="K19" s="27"/>
+      <c r="L19" s="27"/>
+      <c r="M19" s="27"/>
+      <c r="N19" s="27"/>
+    </row>
+    <row r="20" spans="1:18">
+      <c r="A20" s="27"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
       <c r="D20" s="20" t="s">
-        <v>158</v>
-      </c>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28" t="s">
-        <v>155</v>
-      </c>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28">
-        <v>2019</v>
-      </c>
-      <c r="J20" s="28" t="s">
+        <v>157</v>
+      </c>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27">
+        <v>2030</v>
+      </c>
+      <c r="G20" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="K20" s="28">
+      <c r="H20" s="27">
         <v>1</v>
       </c>
-      <c r="L20" s="28">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="M20" s="28">
-        <v>5</v>
-      </c>
-      <c r="N20" s="28" t="s">
-        <v>159</v>
-      </c>
-      <c r="O20" s="28"/>
-      <c r="P20" s="28"/>
-      <c r="Q20" s="28"/>
-    </row>
-    <row r="21" spans="1:21">
-      <c r="A21" s="28"/>
-      <c r="B21" s="28"/>
-      <c r="C21" s="28"/>
+      <c r="I20" s="27">
+        <v>1.67</v>
+      </c>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="27"/>
+      <c r="M20" s="27"/>
+      <c r="N20" s="27"/>
+    </row>
+    <row r="21" spans="1:18">
+      <c r="A21" s="27"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
       <c r="D21" s="20" t="s">
-        <v>158</v>
-      </c>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28" t="s">
-        <v>155</v>
-      </c>
-      <c r="H21" s="28"/>
-      <c r="I21" s="28">
-        <v>2020</v>
-      </c>
-      <c r="J21" s="28" t="s">
+        <v>157</v>
+      </c>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27">
+        <v>2050</v>
+      </c>
+      <c r="G21" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="K21" s="28">
+      <c r="H21" s="27">
         <v>1</v>
       </c>
-      <c r="L21" s="28">
-        <v>1.03</v>
-      </c>
-      <c r="M21" s="3"/>
-      <c r="N21" s="28"/>
-      <c r="O21" s="28"/>
-      <c r="P21" s="28"/>
-      <c r="Q21" s="28"/>
-    </row>
-    <row r="22" spans="1:21">
-      <c r="D22" s="20" t="s">
-        <v>158</v>
-      </c>
-      <c r="G22" s="28" t="s">
-        <v>155</v>
-      </c>
-      <c r="H22" s="28"/>
-      <c r="I22" s="28">
-        <v>2025</v>
-      </c>
-      <c r="J22" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="K22" s="28">
-        <v>1</v>
-      </c>
-      <c r="L22" s="28">
-        <v>2.7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21">
-      <c r="D23" s="20" t="s">
-        <v>158</v>
-      </c>
-      <c r="G23" s="28" t="s">
-        <v>155</v>
-      </c>
-      <c r="H23" s="28"/>
-      <c r="I23" s="28">
-        <v>2030</v>
-      </c>
-      <c r="J23" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="K23" s="28">
-        <v>1</v>
-      </c>
-      <c r="L23">
-        <v>3.78</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" s="28" customFormat="1">
-      <c r="D24" s="20" t="s">
-        <v>158</v>
-      </c>
-      <c r="G24" s="28" t="s">
-        <v>155</v>
-      </c>
-      <c r="I24" s="28">
-        <v>2050</v>
-      </c>
-      <c r="J24" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="K24" s="28">
-        <v>1</v>
-      </c>
-      <c r="L24">
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21">
-      <c r="A26" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="B26" s="28"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="28"/>
-      <c r="J26" s="28"/>
-      <c r="K26" s="28"/>
-      <c r="L26" s="28"/>
-      <c r="M26" s="28"/>
-      <c r="N26" s="28"/>
-      <c r="O26" s="28"/>
-    </row>
-    <row r="27" spans="1:21">
-      <c r="A27" s="28"/>
-      <c r="B27" s="1" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,"~UC_Sets: R_E:",_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,"")))</f>
-        <v>~UC_Sets: R_E: IE,National</v>
-      </c>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="28"/>
-      <c r="K27" s="28"/>
-      <c r="L27" s="28"/>
-      <c r="M27" s="28"/>
-      <c r="N27" s="28"/>
-      <c r="O27" s="28"/>
-    </row>
-    <row r="28" spans="1:21">
-      <c r="A28" s="28"/>
-      <c r="B28" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="28"/>
-      <c r="K28" s="28"/>
-      <c r="L28" s="28"/>
-      <c r="M28" s="28"/>
-      <c r="N28" s="28"/>
-      <c r="O28" s="28"/>
-    </row>
-    <row r="29" spans="1:21">
-      <c r="A29" s="28"/>
-      <c r="B29" s="28"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="28"/>
-      <c r="G29" s="28"/>
-      <c r="H29" s="28"/>
-      <c r="I29" s="28"/>
-      <c r="J29" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="K29" s="28"/>
-      <c r="L29" s="28"/>
-      <c r="M29" s="28"/>
-      <c r="N29" s="28"/>
-      <c r="O29" s="28"/>
-    </row>
-    <row r="30" spans="1:21">
-      <c r="A30" s="28"/>
-      <c r="B30" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I30" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="J30" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="K30" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="L30" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="M30" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="N30" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="O30" s="28"/>
-    </row>
-    <row r="31" spans="1:21">
-      <c r="A31" s="28"/>
-      <c r="B31" s="37" t="s">
-        <v>164</v>
-      </c>
-      <c r="C31" s="28"/>
-      <c r="D31" s="20" t="s">
-        <v>158</v>
-      </c>
-      <c r="E31" s="28"/>
-      <c r="F31" s="28"/>
-      <c r="G31" s="28" t="s">
-        <v>155</v>
-      </c>
-      <c r="H31" s="28"/>
-      <c r="I31" s="28">
-        <v>2020</v>
-      </c>
-      <c r="J31" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="K31" s="28">
-        <v>1</v>
-      </c>
-      <c r="L31" s="28">
-        <v>1</v>
-      </c>
-      <c r="M31" s="28">
-        <v>5</v>
-      </c>
-      <c r="N31" s="28" t="s">
-        <v>159</v>
-      </c>
-      <c r="O31" s="28"/>
-      <c r="S31" s="28"/>
-      <c r="U31" s="26"/>
-    </row>
-    <row r="32" spans="1:21">
-      <c r="A32" s="28"/>
-      <c r="B32" s="28"/>
-      <c r="C32" s="28"/>
-      <c r="D32" s="20" t="s">
-        <v>158</v>
-      </c>
-      <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="28" t="s">
-        <v>155</v>
-      </c>
-      <c r="H32" s="28"/>
-      <c r="I32" s="28">
-        <v>2025</v>
-      </c>
-      <c r="J32" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="K32" s="28">
-        <v>1</v>
-      </c>
-      <c r="L32" s="28">
-        <v>1.67</v>
-      </c>
-      <c r="M32" s="3"/>
-      <c r="N32" s="28"/>
-      <c r="O32" s="28"/>
-      <c r="S32" s="28"/>
-      <c r="U32" s="26"/>
-    </row>
-    <row r="33" spans="1:21">
-      <c r="A33" s="28"/>
-      <c r="B33" s="28"/>
-      <c r="C33" s="28"/>
-      <c r="D33" s="20" t="s">
-        <v>158</v>
-      </c>
-      <c r="E33" s="28"/>
-      <c r="F33" s="28"/>
-      <c r="G33" s="28" t="s">
-        <v>155</v>
-      </c>
-      <c r="H33" s="28"/>
-      <c r="I33" s="28">
-        <v>2030</v>
-      </c>
-      <c r="J33" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="K33" s="28">
-        <v>1</v>
-      </c>
-      <c r="L33" s="28">
-        <v>1.67</v>
-      </c>
-      <c r="M33" s="28"/>
-      <c r="N33" s="28"/>
-      <c r="O33" s="28"/>
-      <c r="S33" s="28"/>
-      <c r="U33" s="26"/>
-    </row>
-    <row r="34" spans="1:21">
-      <c r="A34" s="28"/>
-      <c r="B34" s="28"/>
-      <c r="C34" s="28"/>
-      <c r="D34" s="20" t="s">
-        <v>158</v>
-      </c>
-      <c r="G34" s="28" t="s">
-        <v>155</v>
-      </c>
-      <c r="H34" s="28"/>
-      <c r="I34" s="28">
-        <v>2050</v>
-      </c>
-      <c r="J34" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="K34" s="28">
-        <v>1</v>
-      </c>
-      <c r="L34" s="28">
+      <c r="I21" s="27">
         <v>3.34</v>
       </c>
-      <c r="M34" s="28"/>
-      <c r="N34" s="28"/>
-      <c r="O34" s="28"/>
-      <c r="S34" s="28"/>
-      <c r="U34" s="26"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="27"/>
+      <c r="M21" s="27"/>
+      <c r="N21" s="27"/>
+    </row>
+    <row r="24" spans="1:18" s="27" customFormat="1">
+      <c r="A24"/>
+      <c r="B24"/>
+      <c r="C24"/>
+      <c r="D24"/>
+      <c r="E24"/>
+      <c r="F24"/>
+      <c r="G24"/>
+      <c r="H24"/>
+      <c r="I24"/>
+      <c r="J24"/>
+      <c r="K24"/>
+      <c r="L24"/>
+    </row>
+    <row r="31" spans="1:18">
+      <c r="P31" s="27"/>
+      <c r="R31" s="25"/>
+    </row>
+    <row r="32" spans="1:18">
+      <c r="P32" s="27"/>
+      <c r="R32" s="25"/>
+    </row>
+    <row r="33" spans="16:18">
+      <c r="P33" s="27"/>
+      <c r="R33" s="25"/>
+    </row>
+    <row r="34" spans="16:18">
+      <c r="P34" s="27"/>
+      <c r="R34" s="25"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -4605,7 +4304,7 @@
       </c>
       <c r="J5" s="16"/>
       <c r="K5" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="2:13">
@@ -4630,7 +4329,7 @@
       </c>
       <c r="J6" s="16"/>
       <c r="K6" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="2:13">
@@ -4651,28 +4350,28 @@
         <v>31.1</v>
       </c>
       <c r="K7" s="22" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="2:13" s="28" customFormat="1">
-      <c r="C8" s="28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" s="27" customFormat="1">
+      <c r="C8" s="27" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="28">
+      <c r="E8" s="27">
         <v>0</v>
       </c>
-      <c r="H8" s="28">
+      <c r="H8" s="27">
         <v>5</v>
       </c>
-      <c r="I8" s="28">
+      <c r="I8" s="27">
         <f t="shared" ref="I8" si="1">H8</f>
         <v>5</v>
       </c>
       <c r="K8" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="2:13">
@@ -4745,7 +4444,7 @@
       </c>
       <c r="J12" s="16"/>
       <c r="K12" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="2:13">
@@ -4770,7 +4469,7 @@
       </c>
       <c r="J13" s="16"/>
       <c r="K13" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="2:13">
@@ -4795,34 +4494,34 @@
       </c>
       <c r="J14" s="16"/>
       <c r="K14" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="M14" s="24" t="s">
-        <v>61</v>
+        <v>92</v>
+      </c>
+      <c r="M14" s="23" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="2:13">
-      <c r="C15" s="28" t="s">
+      <c r="C15" s="27" t="s">
         <v>14</v>
       </c>
       <c r="D15" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="28">
+      <c r="E15" s="27">
         <v>0</v>
       </c>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28">
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27">
         <v>5</v>
       </c>
-      <c r="I15" s="28">
+      <c r="I15" s="27">
         <f t="shared" ref="I15" si="3">H15</f>
         <v>5</v>
       </c>
-      <c r="J15" s="28"/>
+      <c r="J15" s="27"/>
       <c r="K15" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M15" s="16">
         <f>2.63*1000/8760/0.3</f>
@@ -4830,7 +4529,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -4843,7 +4542,7 @@
   <dimension ref="A1:V48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:N7"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4873,8 +4572,8 @@
       <c r="B3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="S3" s="25" t="s">
-        <v>62</v>
+      <c r="S3" s="24" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:22">
@@ -4882,12 +4581,12 @@
         <v>7</v>
       </c>
       <c r="S4" t="s">
-        <v>63</v>
-      </c>
-      <c r="U4" s="26">
+        <v>62</v>
+      </c>
+      <c r="U4" s="25">
         <v>0.12</v>
       </c>
-      <c r="V4" s="26">
+      <c r="V4" s="25">
         <v>0.09</v>
       </c>
     </row>
@@ -4932,7 +4631,7 @@
         <v>11</v>
       </c>
       <c r="S5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:22">
@@ -4940,10 +4639,10 @@
         <v>15</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I6">
         <v>2020</v>
@@ -4964,18 +4663,18 @@
         <v>17</v>
       </c>
       <c r="U6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="V6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:22">
       <c r="D7" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I7">
         <v>2050</v>
@@ -4991,24 +4690,24 @@
       </c>
       <c r="M7" s="3"/>
       <c r="S7" t="s">
+        <v>65</v>
+      </c>
+      <c r="T7" t="s">
         <v>66</v>
       </c>
-      <c r="T7" t="s">
+      <c r="U7" t="s">
         <v>67</v>
       </c>
-      <c r="U7" t="s">
-        <v>68</v>
-      </c>
       <c r="V7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:22">
       <c r="S8" t="s">
+        <v>68</v>
+      </c>
+      <c r="T8" t="s">
         <v>69</v>
-      </c>
-      <c r="T8" t="s">
-        <v>70</v>
       </c>
       <c r="U8">
         <v>10127</v>
@@ -5019,10 +4718,10 @@
     </row>
     <row r="9" spans="1:22">
       <c r="S9" t="s">
+        <v>70</v>
+      </c>
+      <c r="T9" t="s">
         <v>71</v>
-      </c>
-      <c r="T9" t="s">
-        <v>72</v>
       </c>
       <c r="U9">
         <v>83</v>
@@ -5033,10 +4732,10 @@
     </row>
     <row r="10" spans="1:22">
       <c r="S10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="T10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="U10">
         <v>56</v>
@@ -5065,10 +4764,10 @@
       <c r="P11" s="12"/>
       <c r="Q11" s="12"/>
       <c r="S11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="T11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="U11">
         <v>56</v>
@@ -5106,10 +4805,10 @@
         <v>3</v>
       </c>
       <c r="S12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="T12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="U12">
         <v>87</v>
@@ -5135,8 +4834,8 @@
         <v>0</v>
       </c>
       <c r="I13" s="17"/>
-      <c r="J13" s="27" t="s">
-        <v>94</v>
+      <c r="J13" s="26" t="s">
+        <v>93</v>
       </c>
       <c r="K13" s="16"/>
       <c r="L13" s="16"/>
@@ -5145,10 +4844,10 @@
       <c r="O13" s="16"/>
       <c r="P13" s="16"/>
       <c r="S13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="T13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="U13">
         <v>108</v>
@@ -5175,10 +4874,10 @@
       <c r="P14" s="16"/>
       <c r="Q14" s="16"/>
       <c r="S14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="T14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="U14">
         <v>108</v>
@@ -5205,10 +4904,10 @@
       <c r="P15" s="16"/>
       <c r="Q15" s="16"/>
       <c r="S15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="T15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="U15">
         <v>108</v>
@@ -5235,10 +4934,10 @@
       <c r="P16" s="16"/>
       <c r="Q16" s="16"/>
       <c r="S16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="T16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="U16">
         <v>37</v>
@@ -5265,10 +4964,10 @@
       <c r="P17" s="16"/>
       <c r="Q17" s="16"/>
       <c r="S17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="T17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="U17">
         <v>25</v>
@@ -5279,10 +4978,10 @@
     </row>
     <row r="18" spans="2:22">
       <c r="S18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="T18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="U18">
         <v>25</v>
@@ -5293,10 +4992,10 @@
     </row>
     <row r="19" spans="2:22">
       <c r="S19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="T19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="U19">
         <v>287</v>
@@ -5307,10 +5006,10 @@
     </row>
     <row r="20" spans="2:22">
       <c r="S20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="T20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="U20">
         <v>66</v>
@@ -5321,10 +5020,10 @@
     </row>
     <row r="21" spans="2:22">
       <c r="S21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="T21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="U21">
         <v>66</v>
@@ -5335,10 +5034,10 @@
     </row>
     <row r="22" spans="2:22">
       <c r="S22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="T22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="U22">
         <v>66</v>
@@ -5349,10 +5048,10 @@
     </row>
     <row r="23" spans="2:22">
       <c r="S23" t="s">
+        <v>85</v>
+      </c>
+      <c r="T23" t="s">
         <v>86</v>
-      </c>
-      <c r="T23" t="s">
-        <v>87</v>
       </c>
       <c r="U23">
         <v>598</v>
@@ -5363,10 +5062,10 @@
     </row>
     <row r="24" spans="2:22">
       <c r="S24" t="s">
+        <v>87</v>
+      </c>
+      <c r="T24" t="s">
         <v>88</v>
-      </c>
-      <c r="T24" t="s">
-        <v>89</v>
       </c>
       <c r="U24">
         <v>7867</v>
@@ -5377,10 +5076,10 @@
     </row>
     <row r="25" spans="2:22">
       <c r="S25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="T25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="U25">
         <v>26</v>
@@ -5391,10 +5090,10 @@
     </row>
     <row r="26" spans="2:22">
       <c r="S26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="T26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="U26">
         <v>458</v>
@@ -5405,32 +5104,32 @@
     </row>
     <row r="28" spans="2:22">
       <c r="U28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="V28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="2:22">
       <c r="S29" t="s">
+        <v>65</v>
+      </c>
+      <c r="T29" t="s">
         <v>66</v>
       </c>
-      <c r="T29" t="s">
+      <c r="U29" t="s">
         <v>67</v>
       </c>
-      <c r="U29" t="s">
-        <v>68</v>
-      </c>
       <c r="V29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="2:22">
       <c r="S30" t="s">
+        <v>68</v>
+      </c>
+      <c r="T30" t="s">
         <v>69</v>
-      </c>
-      <c r="T30" t="s">
-        <v>70</v>
       </c>
       <c r="U30">
         <v>10663</v>
@@ -5441,10 +5140,10 @@
     </row>
     <row r="31" spans="2:22">
       <c r="S31" t="s">
+        <v>70</v>
+      </c>
+      <c r="T31" t="s">
         <v>71</v>
-      </c>
-      <c r="T31" t="s">
-        <v>72</v>
       </c>
       <c r="U31">
         <v>84</v>
@@ -5455,10 +5154,10 @@
     </row>
     <row r="32" spans="2:22">
       <c r="S32" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="T32" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="U32">
         <v>56</v>
@@ -5469,10 +5168,10 @@
     </row>
     <row r="33" spans="19:22">
       <c r="S33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="T33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="U33">
         <v>56</v>
@@ -5483,10 +5182,10 @@
     </row>
     <row r="34" spans="19:22">
       <c r="S34" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="T34" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="U34">
         <v>92</v>
@@ -5497,10 +5196,10 @@
     </row>
     <row r="35" spans="19:22">
       <c r="S35" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="T35" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="U35">
         <v>110</v>
@@ -5511,10 +5210,10 @@
     </row>
     <row r="36" spans="19:22">
       <c r="S36" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="T36" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="U36">
         <v>110</v>
@@ -5525,10 +5224,10 @@
     </row>
     <row r="37" spans="19:22">
       <c r="S37" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="T37" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="U37">
         <v>110</v>
@@ -5539,10 +5238,10 @@
     </row>
     <row r="38" spans="19:22">
       <c r="S38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="T38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="U38">
         <v>37</v>
@@ -5553,10 +5252,10 @@
     </row>
     <row r="39" spans="19:22">
       <c r="S39" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="T39" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="U39">
         <v>25</v>
@@ -5567,10 +5266,10 @@
     </row>
     <row r="40" spans="19:22">
       <c r="S40" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="T40" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="U40">
         <v>25</v>
@@ -5581,10 +5280,10 @@
     </row>
     <row r="41" spans="19:22">
       <c r="S41" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="T41" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="U41">
         <v>291</v>
@@ -5595,10 +5294,10 @@
     </row>
     <row r="42" spans="19:22">
       <c r="S42" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="T42" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="U42">
         <v>68</v>
@@ -5609,10 +5308,10 @@
     </row>
     <row r="43" spans="19:22">
       <c r="S43" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="T43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="U43">
         <v>68</v>
@@ -5623,10 +5322,10 @@
     </row>
     <row r="44" spans="19:22">
       <c r="S44" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="T44" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="U44">
         <v>68</v>
@@ -5637,10 +5336,10 @@
     </row>
     <row r="45" spans="19:22">
       <c r="S45" t="s">
+        <v>85</v>
+      </c>
+      <c r="T45" t="s">
         <v>86</v>
-      </c>
-      <c r="T45" t="s">
-        <v>87</v>
       </c>
       <c r="U45">
         <v>743</v>
@@ -5651,10 +5350,10 @@
     </row>
     <row r="46" spans="19:22">
       <c r="S46" t="s">
+        <v>87</v>
+      </c>
+      <c r="T46" t="s">
         <v>88</v>
-      </c>
-      <c r="T46" t="s">
-        <v>89</v>
       </c>
       <c r="U46">
         <v>8175</v>
@@ -5665,10 +5364,10 @@
     </row>
     <row r="47" spans="19:22">
       <c r="S47" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="T47" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="U47">
         <v>34</v>
@@ -5679,10 +5378,10 @@
     </row>
     <row r="48" spans="19:22">
       <c r="S48" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="T48" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="U48">
         <v>511</v>
@@ -5692,7 +5391,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -5783,10 +5482,10 @@
         <v>18</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I6">
         <v>2020</v>
@@ -5804,15 +5503,15 @@
         <v>15</v>
       </c>
       <c r="N6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:14">
       <c r="D7" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I7">
         <v>2050</v>
@@ -5829,7 +5528,7 @@
       <c r="M7" s="3"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update onshore and offshore wind power potentials and new capacity growth rates
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_PWR_RNW_Potentials.xlsx
+++ b/SuppXLS/Scen_PWR_RNW_Potentials.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_TIMES-Ireland-model\main_PWR_JG\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1131F433-F5DB-4714-8C86-CF1A5241A803}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96AFE408-60E9-409D-BDFE-F9C22826F408}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7875" yWindow="4800" windowWidth="28110" windowHeight="15885" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="6" r:id="rId1"/>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="167">
   <si>
     <t>UC_N</t>
   </si>
@@ -1897,7 +1897,7 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A3:AD37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
@@ -2663,8 +2663,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:M68"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3099,7 +3099,7 @@
         <v>1</v>
       </c>
       <c r="I21" s="27">
-        <v>5.2</v>
+        <v>6.25</v>
       </c>
       <c r="J21" s="27"/>
       <c r="K21" s="27"/>
@@ -3119,7 +3119,7 @@
         <v>1</v>
       </c>
       <c r="I22" s="27">
-        <v>5.5</v>
+        <v>6.6</v>
       </c>
       <c r="K22" s="27"/>
     </row>
@@ -3138,7 +3138,7 @@
         <v>1</v>
       </c>
       <c r="I23" s="27">
-        <v>5.9</v>
+        <v>7</v>
       </c>
       <c r="K23" s="27"/>
     </row>
@@ -3157,7 +3157,7 @@
         <v>1</v>
       </c>
       <c r="I24" s="27">
-        <v>6.9</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="K24" s="27"/>
     </row>
@@ -3319,12 +3319,22 @@
       <c r="A37" s="27"/>
       <c r="B37" s="27"/>
       <c r="C37" s="27"/>
-      <c r="D37" s="20"/>
+      <c r="D37" s="20" t="s">
+        <v>155</v>
+      </c>
       <c r="E37" s="27"/>
-      <c r="F37" s="27"/>
-      <c r="G37" s="27"/>
-      <c r="H37" s="27"/>
-      <c r="I37" s="27"/>
+      <c r="F37" s="27">
+        <v>2050</v>
+      </c>
+      <c r="G37" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="H37" s="27">
+        <v>1</v>
+      </c>
+      <c r="I37" s="27">
+        <v>5</v>
+      </c>
       <c r="J37" s="27"/>
       <c r="K37" s="27"/>
       <c r="L37" s="27"/>
@@ -3417,7 +3427,7 @@
   <dimension ref="A2:W34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3812,7 +3822,7 @@
         <v>1</v>
       </c>
       <c r="I9" s="27">
-        <v>2.7</v>
+        <v>5.4</v>
       </c>
       <c r="N9" t="s">
         <v>45</v>
@@ -3857,7 +3867,7 @@
         <v>1</v>
       </c>
       <c r="I10">
-        <v>3.78</v>
+        <v>7.56</v>
       </c>
       <c r="N10" t="s">
         <v>45</v>
@@ -3905,7 +3915,7 @@
         <v>1</v>
       </c>
       <c r="I11">
-        <v>7.5</v>
+        <v>30</v>
       </c>
       <c r="J11" s="27"/>
       <c r="K11" s="27"/>
@@ -4122,7 +4132,7 @@
         <v>1</v>
       </c>
       <c r="I19" s="27">
-        <v>1.67</v>
+        <v>5</v>
       </c>
       <c r="J19" s="3"/>
       <c r="K19" s="27"/>
@@ -4148,7 +4158,7 @@
         <v>1</v>
       </c>
       <c r="I20" s="27">
-        <v>1.67</v>
+        <v>7.5</v>
       </c>
       <c r="J20" s="27"/>
       <c r="K20" s="27"/>
@@ -4174,7 +4184,7 @@
         <v>1</v>
       </c>
       <c r="I21" s="27">
-        <v>3.34</v>
+        <v>10</v>
       </c>
       <c r="J21" s="27"/>
       <c r="K21" s="27"/>
@@ -4224,7 +4234,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B3:M15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update Wind Onshore and Wind Offshore New Capacity Bound Growth rates to 17.5% onshore and 20% offshore from a seed of 250MW. (Annualised NCAPBND rather than per period results in slower wind deployment in mitigation scenarios)
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_PWR_RNW_Potentials.xlsx
+++ b/SuppXLS/Scen_PWR_RNW_Potentials.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_TIMES-Ireland-model\main_PWR_JG\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_TIMES-Ireland-model\main\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96AFE408-60E9-409D-BDFE-F9C22826F408}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D797763B-6A23-47AC-87D2-E2DB8CC7DFDC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7875" yWindow="4800" windowWidth="28110" windowHeight="15885" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="58410" yWindow="10620" windowWidth="37710" windowHeight="21840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="6" r:id="rId1"/>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="167">
   <si>
     <t>UC_N</t>
   </si>
@@ -175,15 +175,15 @@
   </si>
   <si>
     <t>P-RNW-SOL*</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>P-RNW-HYD*</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>P-RNW-OCE-WAV01</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Country</t>
@@ -359,11 +359,11 @@
   </si>
   <si>
     <t>P-RNW-OCE-TID02</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>P-RNW-SOL-CSP04</t>
     <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>P-RNW-SOL-CSP04</t>
-    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Development</t>
@@ -607,12 +607,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="30">
+  <fonts count="31">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1222,147 +1229,147 @@
   </borders>
   <cellStyleXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1370,29 +1377,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="29" fillId="36" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="36" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="36" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="30" fillId="36" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="37" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="37" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
@@ -1400,6 +1407,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="40">
@@ -2663,8 +2671,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:M68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3311,7 +3319,7 @@
         <v>1</v>
       </c>
       <c r="I36" s="27">
-        <v>2</v>
+        <v>0.61250000000000004</v>
       </c>
       <c r="J36" s="27"/>
     </row>
@@ -3324,7 +3332,7 @@
       </c>
       <c r="E37" s="27"/>
       <c r="F37" s="27">
-        <v>2050</v>
+        <v>2025</v>
       </c>
       <c r="G37" s="27" t="s">
         <v>14</v>
@@ -3333,7 +3341,7 @@
         <v>1</v>
       </c>
       <c r="I37" s="27">
-        <v>5</v>
+        <v>1.37</v>
       </c>
       <c r="J37" s="27"/>
       <c r="K37" s="27"/>
@@ -3344,24 +3352,44 @@
       <c r="A38" s="27"/>
       <c r="B38" s="27"/>
       <c r="C38" s="27"/>
-      <c r="D38" s="20"/>
+      <c r="D38" s="20" t="s">
+        <v>155</v>
+      </c>
       <c r="E38" s="27"/>
-      <c r="F38" s="27"/>
-      <c r="G38" s="27"/>
-      <c r="H38" s="27"/>
-      <c r="I38" s="27"/>
+      <c r="F38" s="27">
+        <v>2030</v>
+      </c>
+      <c r="G38" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="H38" s="27">
+        <v>1</v>
+      </c>
+      <c r="I38" s="27">
+        <v>1</v>
+      </c>
       <c r="J38" s="27"/>
       <c r="K38" s="27"/>
       <c r="L38" s="27"/>
       <c r="M38" s="27"/>
     </row>
     <row r="39" spans="1:13">
-      <c r="D39" s="20"/>
+      <c r="D39" s="20" t="s">
+        <v>155</v>
+      </c>
       <c r="E39" s="27"/>
-      <c r="F39" s="27"/>
-      <c r="G39" s="27"/>
-      <c r="H39" s="27"/>
-      <c r="I39" s="27"/>
+      <c r="F39" s="27">
+        <v>2050</v>
+      </c>
+      <c r="G39" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="H39" s="27">
+        <v>1</v>
+      </c>
+      <c r="I39" s="27">
+        <v>1</v>
+      </c>
       <c r="J39" s="27"/>
       <c r="K39" s="27"/>
       <c r="L39" s="27"/>
@@ -3415,7 +3443,7 @@
       <c r="L68" s="27"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3424,10 +3452,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A2:W34"/>
+  <dimension ref="A2:W57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R50" sqref="R50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4102,7 +4130,7 @@
         <v>1</v>
       </c>
       <c r="I18" s="27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18" s="27">
         <v>5</v>
@@ -4132,7 +4160,7 @@
         <v>1</v>
       </c>
       <c r="I19" s="27">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="J19" s="3"/>
       <c r="K19" s="27"/>
@@ -4158,7 +4186,7 @@
         <v>1</v>
       </c>
       <c r="I20" s="27">
-        <v>7.5</v>
+        <v>0.75</v>
       </c>
       <c r="J20" s="27"/>
       <c r="K20" s="27"/>
@@ -4175,7 +4203,7 @@
       </c>
       <c r="E21" s="27"/>
       <c r="F21" s="27">
-        <v>2050</v>
+        <v>2040</v>
       </c>
       <c r="G21" s="27" t="s">
         <v>14</v>
@@ -4184,7 +4212,7 @@
         <v>1</v>
       </c>
       <c r="I21" s="27">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="J21" s="27"/>
       <c r="K21" s="27"/>
@@ -4192,38 +4220,225 @@
       <c r="M21" s="27"/>
       <c r="N21" s="27"/>
     </row>
+    <row r="22" spans="1:18">
+      <c r="D22" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27">
+        <v>2045</v>
+      </c>
+      <c r="G22" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="27">
+        <v>1</v>
+      </c>
+      <c r="I22" s="27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18">
+      <c r="D23" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27">
+        <v>2050</v>
+      </c>
+      <c r="G23" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="27">
+        <v>1</v>
+      </c>
+      <c r="I23" s="27">
+        <v>3</v>
+      </c>
+    </row>
     <row r="24" spans="1:18" s="27" customFormat="1">
       <c r="A24"/>
       <c r="B24"/>
       <c r="C24"/>
-      <c r="D24"/>
-      <c r="E24"/>
-      <c r="F24"/>
-      <c r="G24"/>
-      <c r="H24"/>
-      <c r="I24"/>
+      <c r="D24" s="20"/>
       <c r="J24"/>
       <c r="K24"/>
       <c r="L24"/>
+      <c r="N24" s="37"/>
+    </row>
+    <row r="25" spans="1:18">
+      <c r="D25" s="20"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="27"/>
+      <c r="I25" s="27"/>
+    </row>
+    <row r="26" spans="1:18">
+      <c r="D26" s="20"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="27"/>
+      <c r="I26" s="27"/>
+    </row>
+    <row r="28" spans="1:18">
+      <c r="M28" s="27"/>
+      <c r="N28" s="27"/>
+    </row>
+    <row r="29" spans="1:18">
+      <c r="M29" s="27"/>
+      <c r="N29" s="27"/>
+    </row>
+    <row r="30" spans="1:18">
+      <c r="M30" s="27"/>
+      <c r="N30" s="27"/>
     </row>
     <row r="31" spans="1:18">
+      <c r="L31" s="27"/>
+      <c r="M31" s="27"/>
+      <c r="N31" s="27"/>
       <c r="P31" s="27"/>
       <c r="R31" s="25"/>
     </row>
     <row r="32" spans="1:18">
+      <c r="L32" s="27"/>
+      <c r="M32" s="27"/>
+      <c r="N32" s="27"/>
       <c r="P32" s="27"/>
       <c r="R32" s="25"/>
     </row>
-    <row r="33" spans="16:18">
+    <row r="33" spans="12:18">
+      <c r="L33" s="27"/>
+      <c r="M33" s="27"/>
+      <c r="N33" s="27"/>
       <c r="P33" s="27"/>
       <c r="R33" s="25"/>
     </row>
-    <row r="34" spans="16:18">
+    <row r="34" spans="12:18">
+      <c r="L34" s="27"/>
+      <c r="M34" s="27"/>
+      <c r="N34" s="27"/>
       <c r="P34" s="27"/>
       <c r="R34" s="25"/>
     </row>
+    <row r="35" spans="12:18">
+      <c r="L35" s="27"/>
+      <c r="M35" s="27"/>
+      <c r="N35" s="27"/>
+    </row>
+    <row r="36" spans="12:18">
+      <c r="L36" s="27"/>
+      <c r="M36" s="27"/>
+      <c r="N36" s="27"/>
+    </row>
+    <row r="37" spans="12:18">
+      <c r="L37" s="27"/>
+      <c r="M37" s="27"/>
+      <c r="N37" s="27"/>
+    </row>
+    <row r="38" spans="12:18">
+      <c r="L38" s="27"/>
+      <c r="M38" s="27"/>
+      <c r="N38" s="27"/>
+    </row>
+    <row r="39" spans="12:18">
+      <c r="L39" s="27"/>
+      <c r="M39" s="27"/>
+      <c r="N39" s="27"/>
+    </row>
+    <row r="40" spans="12:18">
+      <c r="L40" s="27"/>
+      <c r="M40" s="27"/>
+      <c r="N40" s="27"/>
+    </row>
+    <row r="41" spans="12:18">
+      <c r="L41" s="27"/>
+      <c r="M41" s="27"/>
+      <c r="N41" s="27"/>
+    </row>
+    <row r="42" spans="12:18">
+      <c r="L42" s="27"/>
+      <c r="M42" s="27"/>
+      <c r="N42" s="27"/>
+    </row>
+    <row r="43" spans="12:18">
+      <c r="L43" s="27"/>
+      <c r="M43" s="27"/>
+      <c r="N43" s="27"/>
+    </row>
+    <row r="44" spans="12:18">
+      <c r="L44" s="27"/>
+      <c r="M44" s="27"/>
+      <c r="N44" s="27"/>
+    </row>
+    <row r="45" spans="12:18">
+      <c r="L45" s="27"/>
+      <c r="M45" s="27"/>
+      <c r="N45" s="27"/>
+    </row>
+    <row r="46" spans="12:18">
+      <c r="L46" s="27"/>
+      <c r="M46" s="27"/>
+      <c r="N46" s="27"/>
+    </row>
+    <row r="47" spans="12:18">
+      <c r="L47" s="27"/>
+      <c r="M47" s="27"/>
+      <c r="N47" s="27"/>
+    </row>
+    <row r="48" spans="12:18">
+      <c r="L48" s="27"/>
+      <c r="M48" s="27"/>
+      <c r="N48" s="27"/>
+    </row>
+    <row r="49" spans="12:14">
+      <c r="L49" s="27"/>
+      <c r="M49" s="27"/>
+      <c r="N49" s="27"/>
+    </row>
+    <row r="50" spans="12:14">
+      <c r="L50" s="27"/>
+      <c r="M50" s="27"/>
+      <c r="N50" s="27"/>
+    </row>
+    <row r="51" spans="12:14">
+      <c r="L51" s="27"/>
+      <c r="M51" s="27"/>
+      <c r="N51" s="27"/>
+    </row>
+    <row r="52" spans="12:14">
+      <c r="L52" s="27"/>
+      <c r="M52" s="27"/>
+      <c r="N52" s="27"/>
+    </row>
+    <row r="53" spans="12:14">
+      <c r="L53" s="27"/>
+      <c r="M53" s="27"/>
+      <c r="N53" s="27"/>
+    </row>
+    <row r="54" spans="12:14">
+      <c r="L54" s="27"/>
+      <c r="M54" s="27"/>
+      <c r="N54" s="27"/>
+    </row>
+    <row r="55" spans="12:14">
+      <c r="L55" s="27"/>
+      <c r="M55" s="27"/>
+      <c r="N55" s="27"/>
+    </row>
+    <row r="56" spans="12:14">
+      <c r="L56" s="27"/>
+      <c r="M56" s="27"/>
+      <c r="N56" s="27"/>
+    </row>
+    <row r="57" spans="12:14">
+      <c r="L57" s="27"/>
+      <c r="M57" s="27"/>
+      <c r="N57" s="27"/>
+    </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -4539,7 +4754,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -5401,7 +5616,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -5538,7 +5753,7 @@
       <c r="M7" s="3"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>